<commit_message>
Serie Adivina Cuánto te Quiero SD y HD
</commit_message>
<xml_diff>
--- a/XML_SD_HD.xlsx
+++ b/XML_SD_HD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Readfile\createReadFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58D3F44F-F490-4D66-88CD-317E2C82BA12}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA739AEF-7234-4E8F-9C79-06325B3AA408}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1516" uniqueCount="282">
   <si>
     <t>Creation_Date</t>
   </si>
@@ -261,388 +261,622 @@
     <t>EP 20</t>
   </si>
   <si>
-    <t>EEDATG111_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEDA6000000000000111</t>
-  </si>
-  <si>
-    <t>Serie Daniel Tigre</t>
-  </si>
-  <si>
-    <t>Daniel TigreT01EP11</t>
-  </si>
-  <si>
-    <t>Daniel Tigre T01 EP11</t>
-  </si>
-  <si>
-    <t>Edye presenta: Daniel visita a la Srita. Elena su casa es un museo carrusel. Juntos juegan a ser astronautas.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Daniel visita a la Srita. Elena cuya casa es un museo carrusel. Juntos jugarán a ser astronautas para volar al espacio exterior. Pero ocurre un contratiempo: el telescopio se ha dañado.</t>
-  </si>
-  <si>
-    <t>Infantil/Daniel Tigre</t>
-  </si>
-  <si>
-    <t>Daniel Tigre</t>
-  </si>
-  <si>
-    <t>Jake Bale, Tomy Lioutas, Heather Bambrick , Ted Dykstra</t>
-  </si>
-  <si>
-    <t>Striped Tiger, LLC</t>
-  </si>
-  <si>
-    <t>Bale Jake, Lioutas Tomy, Bambrick Heather, Dykstra Ted</t>
-  </si>
-  <si>
-    <t>Kapridov, Vadim</t>
-  </si>
-  <si>
-    <t>EEDATG111.mpg</t>
-  </si>
-  <si>
-    <t>EEDATG1_box.jpg</t>
-  </si>
-  <si>
-    <t>EEDATG111_land.jpg</t>
-  </si>
-  <si>
-    <t>EEDATG112_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEDA6000000000000112</t>
-  </si>
-  <si>
-    <t>Daniel TigreT01EP12</t>
-  </si>
-  <si>
-    <t>Daniel Tigre T01 EP12</t>
-  </si>
-  <si>
-    <t>Edye presenta: Daniel visita el castillo del Príncipe Miércoles, quien le muestra su colección de piedras.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Daniel va a jugar al castillo de su amigo Príncipe Miércoles, quien lo invita a conocer su colección de piedras. Pero hay un problema…no pueden jugar con ellas.</t>
-  </si>
-  <si>
-    <t>EEDATG112.mpg</t>
-  </si>
-  <si>
-    <t>EEDATG112_land.jpg</t>
-  </si>
-  <si>
-    <t>EEDATG113_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEDA6000000000000113</t>
-  </si>
-  <si>
-    <t>Daniel TigreT01EP13</t>
-  </si>
-  <si>
-    <t>Daniel Tigre T01 EP13</t>
-  </si>
-  <si>
-    <t>Edye presenta: Daniel va a jugar a casa de Catalina. Donde organizan una fiesta de cumpleaños para el Sr. Mono</t>
-  </si>
-  <si>
-    <t>Edye presenta: Hoy Daniel va a jugar a la casa de Catalina gatita. Organizan una fiesta de cumpleaños para el señor Mono. Todos los peluches están invitados a la fiesta. Pero surge un inconveniente. ¿Podrán los amigos ayudarse para solucionarlo?</t>
-  </si>
-  <si>
-    <t>EEDATG113.mpg</t>
-  </si>
-  <si>
-    <t>EEDATG113_land.jpg</t>
-  </si>
-  <si>
-    <t>EEDATG114_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEDA6000000000000114</t>
-  </si>
-  <si>
-    <t>Daniel TigreT01EP14</t>
-  </si>
-  <si>
-    <t>Daniel Tigre T01 EP14</t>
-  </si>
-  <si>
-    <t>Edye presenta: En la biblioteca de Úo, Daniel y su amigo crean su propio final de una historia de dinosaurios.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Daniel visita a su amigo Úo el búho, quien lo invita jugar en su biblioteca. Juntos compartirán la lectura de un libro de dinosaurios, pero les falta la última página entonces tendrán que crear su propio final.</t>
-  </si>
-  <si>
-    <t>EEDATG114.mpg</t>
-  </si>
-  <si>
-    <t>EEDATG114_land.jpg</t>
-  </si>
-  <si>
-    <t>EEDATG115_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEDA6000000000000115</t>
-  </si>
-  <si>
-    <t>Daniel TigreT01EP15</t>
-  </si>
-  <si>
-    <t>Daniel Tigre T01 EP15</t>
-  </si>
-  <si>
-    <t>Edye presenta: Daniel decide sorprender a su papá enviándole una carta con un dibujo.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Despúes de que Daniel y su papá reciben una carta del abuelo Tigre. Daniel decide sorpender a su papá enviándole una carta con un dibujo, por lo cual en compañía de su mamá va a la oficina de correo a depositarla.</t>
-  </si>
-  <si>
-    <t>EEDATG115.mpg</t>
-  </si>
-  <si>
-    <t>EEDATG115_land.jpg</t>
-  </si>
-  <si>
-    <t>EEDATG116_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEDA6000000000000116</t>
-  </si>
-  <si>
-    <t>Daniel TigreT01EP16</t>
-  </si>
-  <si>
-    <t>Daniel Tigre T01 EP16</t>
-  </si>
-  <si>
-    <t>Edye presenta: Daniel y su papá deciden soprender a mamá con un pan de banana elaborado por ellos mismos.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Daniel juega con su mamá, a quien decide hacerle un collar. Después junto con su papá van a la panadería para prepararle un pan de banana y sorprenderla.</t>
-  </si>
-  <si>
-    <t>EEDATG116.mpg</t>
-  </si>
-  <si>
-    <t>EEDATG116_land.jpg</t>
-  </si>
-  <si>
-    <t>EEDATG117_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEDA6000000000000117</t>
-  </si>
-  <si>
-    <t>Daniel TigreT01EP17</t>
-  </si>
-  <si>
-    <t>Daniel Tigre T01 EP17</t>
-  </si>
-  <si>
-    <t>Edye presenta: La mamá quiere hacer panqueques de fresas, así que van al Jardín Encantado a recolectarlas.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Daniel comienza el día haciendo ejercicios de estiramiento. La mamá quiere hacer panqueques de fresas, pero como no tienen fruta deben ir al Jardín Encantado a recolectarlas para acabar de preparar el desayuno.</t>
-  </si>
-  <si>
-    <t>EEDATG117.mpg</t>
-  </si>
-  <si>
-    <t>EEDATG117_land.jpg</t>
-  </si>
-  <si>
-    <t>EEDATG118_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEDA6000000000000118</t>
-  </si>
-  <si>
-    <t>Daniel TigreT01EP18</t>
-  </si>
-  <si>
-    <t>Daniel Tigre T01 EP18</t>
-  </si>
-  <si>
-    <t>Edye presenta: Daniel y sus amigas visitan la fábrica de crayones para conocer como se elaboran.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Daniel y sus amigas Elena y Catalina, visitan la fábrica de crayones para conocer como se elaboran.</t>
-  </si>
-  <si>
-    <t>EEDATG118.mpg</t>
-  </si>
-  <si>
-    <t>EEDATG118_land.jpg</t>
-  </si>
-  <si>
-    <t>EEDATG119_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEDA6000000000000119</t>
-  </si>
-  <si>
-    <t>Daniel TigreT01EP19</t>
-  </si>
-  <si>
-    <t>Daniel Tigre T01 EP19</t>
-  </si>
-  <si>
-    <t>Edye presenta: Daniel compartirá con sus amigos su nuevo juguete el auto tigre-tástico.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Hoy Daniel tiene una sorpresa para sus amigos compartirá con ellos su nuevo juguete el auto tigre-tástico. Su papá lo acompaña al parque donde se encontrará con sus amigos, quienes también llevarán sus juguetes. Todos comparten sus autos.</t>
-  </si>
-  <si>
-    <t>EEDATG119.mpg</t>
-  </si>
-  <si>
-    <t>EEDATG119_land.jpg</t>
-  </si>
-  <si>
-    <t>EEDATG120_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEDA6000000000000120</t>
-  </si>
-  <si>
-    <t>Daniel TigreT01EP20</t>
-  </si>
-  <si>
-    <t>Daniel Tigre T01 EP20</t>
-  </si>
-  <si>
-    <t>Edye presenta: Daniel y Catalina preparan un baile de la selva. Daniel será un león y su amiga una bella flor.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Daniel y Catalina preparan un show del baile de la selva. Daniel elige ser el gran león de la selva y su amiga una flor. Ambos compartirán el tutu para su presentación.</t>
-  </si>
-  <si>
-    <t>EEDATG120.mpg</t>
-  </si>
-  <si>
-    <t>EEDATG120_land.jpg</t>
-  </si>
-  <si>
-    <t>EEDATG111_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEDA7000000000000111</t>
-  </si>
-  <si>
-    <t>Daniel Tigre T01 EP11 HD</t>
-  </si>
-  <si>
-    <t>EEDATG111.ts</t>
-  </si>
-  <si>
-    <t>EEDATG112_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEDA7000000000000112</t>
-  </si>
-  <si>
-    <t>Daniel Tigre T01 EP12 HD</t>
-  </si>
-  <si>
-    <t>EEDATG112.ts</t>
-  </si>
-  <si>
-    <t>EEDATG113_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEDA7000000000000113</t>
-  </si>
-  <si>
-    <t>Daniel Tigre T01 EP13 HD</t>
-  </si>
-  <si>
-    <t>EEDATG113.ts</t>
-  </si>
-  <si>
-    <t>EEDATG114_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEDA7000000000000114</t>
-  </si>
-  <si>
-    <t>Daniel Tigre T01 EP14 HD</t>
-  </si>
-  <si>
-    <t>EEDATG114.ts</t>
-  </si>
-  <si>
-    <t>EEDATG115_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEDA7000000000000115</t>
-  </si>
-  <si>
-    <t>Daniel Tigre T01 EP15 HD</t>
-  </si>
-  <si>
-    <t>EEDATG115.ts</t>
-  </si>
-  <si>
-    <t>EEDATG116_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEDA7000000000000116</t>
-  </si>
-  <si>
-    <t>Daniel Tigre T01 EP16 HD</t>
-  </si>
-  <si>
-    <t>EEDATG116.ts</t>
-  </si>
-  <si>
-    <t>EEDATG117_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEDA7000000000000117</t>
-  </si>
-  <si>
-    <t>Daniel Tigre T01 EP17 HD</t>
-  </si>
-  <si>
-    <t>EEDATG117.ts</t>
-  </si>
-  <si>
-    <t>EEDATG118_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEDA7000000000000118</t>
-  </si>
-  <si>
-    <t>Daniel Tigre T01 EP18 HD</t>
-  </si>
-  <si>
-    <t>EEDATG118.ts</t>
-  </si>
-  <si>
-    <t>EEDATG119_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEDA7000000000000119</t>
-  </si>
-  <si>
-    <t>Daniel Tigre T01 EP19 HD</t>
-  </si>
-  <si>
-    <t>EEDATG119.ts</t>
-  </si>
-  <si>
-    <t>EEDATG120_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEDA7000000000000120</t>
-  </si>
-  <si>
-    <t>Daniel Tigre T01 EP20 HD</t>
-  </si>
-  <si>
-    <t>EEDATG120.ts</t>
+    <t>EEGHML111_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEGH6000000000000111</t>
+  </si>
+  <si>
+    <t>Serie Adivina Cuánto te Quiero</t>
+  </si>
+  <si>
+    <t>Adivina Cuánto te QuieroT01EP11</t>
+  </si>
+  <si>
+    <t>Adivina Cuánto te Quiero T01 EP11</t>
+  </si>
+  <si>
+    <t>Edye presenta: Una simpática mariquita pasa el día con Nutbrown , cuando se marcha él descubre algo hermoso.</t>
+  </si>
+  <si>
+    <t>Edye presenta: Una linda mariquita manchada aterriza en Nutbrown y se queda con él. Todos sus amigos la admiran y él se siente muy especial. Pero de pronto la mariquita vuela, Nutbrown la sigue y descubre que tiene muchos bebés pequeños y manchados esperándola.</t>
+  </si>
+  <si>
+    <t>Infantil/Adivina Cuánto te Quiero</t>
+  </si>
+  <si>
+    <t>Adivina Cuánto te Quiero</t>
+  </si>
+  <si>
+    <t>Matthew Jacob Wayne, Allie Carlton , Kirk Thornton, Kat Cressida, Stuart Allan, Nick Roye, Bianca Mercado, Michaela Dean, Angie Perron</t>
+  </si>
+  <si>
+    <t>SLR Productions</t>
+  </si>
+  <si>
+    <t>Wayne Matthew Jacob, Carlton Allie, Thornton Kirk, Cressida Kat, Allan Stuart, Roye Nick, Mercado Bianca, Dean Michaela, Perron Angie</t>
+  </si>
+  <si>
+    <t>Moltzen, Steve</t>
+  </si>
+  <si>
+    <t>EEGHML111.mpg</t>
+  </si>
+  <si>
+    <t>EEGHML1_box.jpg</t>
+  </si>
+  <si>
+    <t>EEGHML111_land.jpg</t>
+  </si>
+  <si>
+    <t>EEGHML112_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEGH6000000000000112</t>
+  </si>
+  <si>
+    <t>Adivina Cuánto te QuieroT01EP12</t>
+  </si>
+  <si>
+    <t>Adivina Cuánto te Quiero T01 EP12</t>
+  </si>
+  <si>
+    <t>Edye presenta: La lluvia parece arruinar el día de Nutbrown y Ratoncita ¿Dejarán de divertirse por el agua?</t>
+  </si>
+  <si>
+    <t>Edye presenta: Nutbrown y Ratoncita disfrutan de un día soleado en la pradera hasta que la lluvia los obliga a buscar refugio. ¿Permitirán los amigos que un poco de agua arruine su diversión o descubrirán que los días lluviosos pueden ser igual de emocionantes?</t>
+  </si>
+  <si>
+    <t>EEGHML112.mpg</t>
+  </si>
+  <si>
+    <t>EEGHML112_land.jpg</t>
+  </si>
+  <si>
+    <t>EEGHML113_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEGH6000000000000113</t>
+  </si>
+  <si>
+    <t>Adivina Cuánto te QuieroT01EP13</t>
+  </si>
+  <si>
+    <t>Adivina Cuánto te Quiero T01 EP13</t>
+  </si>
+  <si>
+    <t>Edye presenta: ¡Las hormigas robaron las bayas de Nutbrown! Pero entiende las razones por las que lo hicieron.</t>
+  </si>
+  <si>
+    <t>Edye presenta: Nutbrown está enojado porque las hormigas se llevaron sus bayas. Pápa Nutbrown le explica que las hormigas probablemente estaban llevando las bayas a sus familias, Nutbrown las perdona y descubre que son muy inteligentes y quiere ser como ellas.</t>
+  </si>
+  <si>
+    <t>EEGHML113.mpg</t>
+  </si>
+  <si>
+    <t>EEGHML113_land.jpg</t>
+  </si>
+  <si>
+    <t>EEGHML114_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEGH6000000000000114</t>
+  </si>
+  <si>
+    <t>Adivina Cuánto te QuieroT01EP14</t>
+  </si>
+  <si>
+    <t>Adivina Cuánto te Quiero T01 EP14</t>
+  </si>
+  <si>
+    <t>Edye presenta: Nutbrown y Ratoncita buscan “tesoros azules” pero Papá Nutbrown encuentra el mejor de todos.</t>
+  </si>
+  <si>
+    <t>Edye presenta: Nutbrown encuentra una hermosa mariposa azul y va con Ratoncita a buscar otros tesoros azules que incluyen arándanos, campanas azules e incluso cáscaras de huevo azules. Pero Papá Nutbrown ha descubierto el tesoro azul más grande de todos. ¿Qué será?</t>
+  </si>
+  <si>
+    <t>EEGHML114.mpg</t>
+  </si>
+  <si>
+    <t>EEGHML114_land.jpg</t>
+  </si>
+  <si>
+    <t>EEGHML115_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEGH6000000000000115</t>
+  </si>
+  <si>
+    <t>Adivina Cuánto te QuieroT01EP15</t>
+  </si>
+  <si>
+    <t>Adivina Cuánto te Quiero T01 EP15</t>
+  </si>
+  <si>
+    <t>Edye presenta: Tras conocer las diferentes y hermosas casas de sus amigos, ¿Qué pensará Nutbrown de la suya?</t>
+  </si>
+  <si>
+    <t>Edye presenta: Papá Nutbrown envía al pequeño Nutbrown a invitar a sus amigos a desayunar. En el camino, Nutbrown descubre lo maravillosas y diferentes que son todas las casas de sus amigos. Tras conocer las de los demás ¿Su casa le seguirá pareciendo hermosa?</t>
+  </si>
+  <si>
+    <t>EEGHML115.mpg</t>
+  </si>
+  <si>
+    <t>EEGHML115_land.jpg</t>
+  </si>
+  <si>
+    <t>EEGHML116_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEGH6000000000000116</t>
+  </si>
+  <si>
+    <t>Adivina Cuánto te QuieroT01EP16</t>
+  </si>
+  <si>
+    <t>Adivina Cuánto te Quiero T01 EP16</t>
+  </si>
+  <si>
+    <t>Edye presenta: Nutbrown quiere una cola larga e inteligente hasta que descubre que la suya es lo que necesita.</t>
+  </si>
+  <si>
+    <t>Edye presenta: Nutbrown decide que quiere una cola larga e inteligente como sus amigos, en lugar de una corta y esponjosa. Cuando Papá Nutbrown ve a su hijo en un campo cubierto de hierba, se dan cuenta de que la pequeña cola de Nutbrown es inteligente a su manera.</t>
+  </si>
+  <si>
+    <t>EEGHML116.mpg</t>
+  </si>
+  <si>
+    <t>EEGHML116_land.jpg</t>
+  </si>
+  <si>
+    <t>EEGHML117_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEGH6000000000000117</t>
+  </si>
+  <si>
+    <t>Adivina Cuánto te QuieroT01EP17</t>
+  </si>
+  <si>
+    <t>Adivina Cuánto te Quiero T01 EP17</t>
+  </si>
+  <si>
+    <t>Edye presenta: Nutbrown toma “la cosa favorita” de Ratoncita y la pierde ¿Cómo podrá explicarle lo que pasó?</t>
+  </si>
+  <si>
+    <t>Edye presenta: Ratoncita está emocionada y quiere mostrarle a Nutbrown su nueva cosa favorita, una flor, ¡la más bonita de todas! La liebre la toma para enseñársela a su papá, pero la flor desaparece durante la noche,¿Cómo podrá Nutbrown explicarlo a Ratoncita?</t>
+  </si>
+  <si>
+    <t>EEGHML117.mpg</t>
+  </si>
+  <si>
+    <t>EEGHML117_land.jpg</t>
+  </si>
+  <si>
+    <t>EEGHML118_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEGH6000000000000118</t>
+  </si>
+  <si>
+    <t>Adivina Cuánto te QuieroT01EP18</t>
+  </si>
+  <si>
+    <t>Adivina Cuánto te Quiero T01 EP18</t>
+  </si>
+  <si>
+    <t>Edye presenta: Nutbrown y su padre comienzan a seguir los palos que flotan en el río ¿A dónde terminarán?</t>
+  </si>
+  <si>
+    <t>Edye presenta: Nutbrown y su padre notan que los palos flotan en el agua. Intrigados, comienzan a seguirlos río abajo para ver a dónde van. La persecusión no es fácil pero encuentran una sorpresa en cada esquina, pero ¿Dónde terminarán los palos?</t>
+  </si>
+  <si>
+    <t>EEGHML118.mpg</t>
+  </si>
+  <si>
+    <t>EEGHML118_land.jpg</t>
+  </si>
+  <si>
+    <t>EEGHML119_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEGH6000000000000119</t>
+  </si>
+  <si>
+    <t>Adivina Cuánto te QuieroT01EP19</t>
+  </si>
+  <si>
+    <t>Adivina Cuánto te Quiero T01 EP19</t>
+  </si>
+  <si>
+    <t>Edye presenta: Ardilla Gris le da un regalo a Nutbrown pero luego se lo quita. ¿Podrán superar el problema?</t>
+  </si>
+  <si>
+    <t>Edye presenta: En un día caluroso, Ardilla gris ofrece a Nutbrown y Ratoncita un regalo: grandes sombrillas. Más tarde cambia de opinión y le pide a Nutbrown que devuelva la suya, lo que lo entristece. ¿Podrán encontrar la manera de que todos estén contentos?</t>
+  </si>
+  <si>
+    <t>EEGHML119.mpg</t>
+  </si>
+  <si>
+    <t>EEGHML119_land.jpg</t>
+  </si>
+  <si>
+    <t>EEGHML120_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEGH6000000000000120</t>
+  </si>
+  <si>
+    <t>Adivina Cuánto te QuieroT01EP20</t>
+  </si>
+  <si>
+    <t>Adivina Cuánto te Quiero T01 EP20</t>
+  </si>
+  <si>
+    <t>Edye presenta: Nutbrown quiere ser como su papá. Aunque ¡él también tiene algunos trucos que enseñarle!</t>
+  </si>
+  <si>
+    <t>Edye presenta: Papá Nutbrown sabe todos los trucos y escondites para encontrar golosinas y el pequeño Nutbrown quisiera ser tan inteligente como su padre. Sin embargo, pronto descubre que hay algunas cosas que una liebre pequeña puede enseñar a una liebre grande.</t>
+  </si>
+  <si>
+    <t>EEGHML120.mpg</t>
+  </si>
+  <si>
+    <t>EEGHML120_land.jpg</t>
+  </si>
+  <si>
+    <t>EEGHML121_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEGH6000000000000121</t>
+  </si>
+  <si>
+    <t>Adivina Cuánto te QuieroT01EP21</t>
+  </si>
+  <si>
+    <t>Adivina Cuánto te Quiero T01 EP21</t>
+  </si>
+  <si>
+    <t>EP 21</t>
+  </si>
+  <si>
+    <t>Edye presenta: Hace mucho calor. Nutbrown y sus amigos le piden a Búho Blanco un cuento muy frío para dormir.</t>
+  </si>
+  <si>
+    <t>Edye presenta: En una noche más calurosa del verano, Nutbrown y sus amigos no pueden dormir y le piden a Búho Blanco que les cuente un cuento muy frío. ¿Se le ocurrirá una historia que pueda hacer que se sientan geniales y finalmente los haga dormir?</t>
+  </si>
+  <si>
+    <t>EEGHML121.mpg</t>
+  </si>
+  <si>
+    <t>EEGHML121_land.jpg</t>
+  </si>
+  <si>
+    <t>EEGHML122_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEGH6000000000000122</t>
+  </si>
+  <si>
+    <t>Adivina Cuánto te QuieroT01EP22</t>
+  </si>
+  <si>
+    <t>Adivina Cuánto te Quiero T01 EP22</t>
+  </si>
+  <si>
+    <t>EP 22</t>
+  </si>
+  <si>
+    <t>Edye presenta: Nutbrown descubre que cada criatura tiene una visión personal de lo que hay a su alrededor.</t>
+  </si>
+  <si>
+    <t>Edye presenta: Nutbrown queda impresionado por la descripción de Pajarita Azul de un campo florido que se ve como un mar de color desde las alturas. De visita el campo con Papá Nutbrown y Ratoncita, descubre que cada uno tiene su propia y única visión del lugar.</t>
+  </si>
+  <si>
+    <t>EEGHML122.mpg</t>
+  </si>
+  <si>
+    <t>EEGHML122_land.jpg</t>
+  </si>
+  <si>
+    <t>EEGHML123_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEGH6000000000000123</t>
+  </si>
+  <si>
+    <t>Adivina Cuánto te QuieroT01EP23</t>
+  </si>
+  <si>
+    <t>Adivina Cuánto te Quiero T01 EP23</t>
+  </si>
+  <si>
+    <t>EP 23</t>
+  </si>
+  <si>
+    <t>Edye presenta: Nutbrown decide inventar una historia, pero le resulta más difícil de lo que pensaba.</t>
+  </si>
+  <si>
+    <t>Edye presenta: Tras escuchar una historia del Búho Blanco, Nutbrown decide inventar una historia, pero le resulta más difícil de lo que pensaba. Con la ayuda de su padre, usa un poco de fruta que ha recogido en el camino para ayudarlo a contar una gran historia.</t>
+  </si>
+  <si>
+    <t>EEGHML123.mpg</t>
+  </si>
+  <si>
+    <t>EEGHML123_land.jpg</t>
+  </si>
+  <si>
+    <t>EEGHML124_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEGH6000000000000124</t>
+  </si>
+  <si>
+    <t>Adivina Cuánto te QuieroT01EP24</t>
+  </si>
+  <si>
+    <t>Adivina Cuánto te Quiero T01 EP24</t>
+  </si>
+  <si>
+    <t>EP 24</t>
+  </si>
+  <si>
+    <t>Edye presenta: Nutbrown y su papá intercambian sus roles jugando. Pronto descubren que es mejor ser uno mismo.</t>
+  </si>
+  <si>
+    <t>Edye presenta: Por un día, Nutbrown ocupará el lugar y las actividades de su papá mientras Papá Nutbrown actuará como su hijo jugando con sus amigos. Todo es muy divertido hasta que se dan cuenta de que son mucho, mucho mejores, siendo ellos mismos.</t>
+  </si>
+  <si>
+    <t>EEGHML124.mpg</t>
+  </si>
+  <si>
+    <t>EEGHML124_land.jpg</t>
+  </si>
+  <si>
+    <t>EEGHML125_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEGH6000000000000125</t>
+  </si>
+  <si>
+    <t>Adivina Cuánto te QuieroT01EP25</t>
+  </si>
+  <si>
+    <t>Adivina Cuánto te Quiero T01 EP25</t>
+  </si>
+  <si>
+    <t>EP 25</t>
+  </si>
+  <si>
+    <t>Edye presenta: Nutbrown se pregunta si es posible disfrutar una tormenta y de las maravillas de la naturaleza.</t>
+  </si>
+  <si>
+    <t>Edye presenta: Una tormenta obliga a Nutbrown y sus amigos a refugiarse en una cueva. Ahí Papá Nutbrown les explica que los ruidos no pueden lastimarte, pero ¿los ayudará a superar sus miedos como para disfrutar de la tormenta y las maravillas de la naturaleza?</t>
+  </si>
+  <si>
+    <t>EEGHML125.mpg</t>
+  </si>
+  <si>
+    <t>EEGHML125_land.jpg</t>
+  </si>
+  <si>
+    <t>EEGHML126_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEGH6000000000000126</t>
+  </si>
+  <si>
+    <t>Adivina Cuánto te QuieroT01EP26</t>
+  </si>
+  <si>
+    <t>Adivina Cuánto te Quiero T01 EP26</t>
+  </si>
+  <si>
+    <t>EP 26</t>
+  </si>
+  <si>
+    <t>Edye presenta: Nutbrown y sus amigos descubren un árbol lleno ciruelas ¿qué pasará cuando se acaben?</t>
+  </si>
+  <si>
+    <t>Edye presenta: En verano Nutbrown descubre un árbol lleno ciruelas. Pero él no es el único que disfruta de la fruta: todos los animales de la pradera vienen probarla. Cuando avanza el verano, Nutbrown se pregunta ¿qué harán todos los animales cuando se terminen?</t>
+  </si>
+  <si>
+    <t>EEGHML126.mpg</t>
+  </si>
+  <si>
+    <t>EEGHML126_land.jpg</t>
+  </si>
+  <si>
+    <t>EEGHML111_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEGH7000000000000111</t>
+  </si>
+  <si>
+    <t>Adivina Cuánto te Quiero T01 EP11 HD</t>
+  </si>
+  <si>
+    <t>EEGHML111.ts</t>
+  </si>
+  <si>
+    <t>EEGHML112_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEGH7000000000000112</t>
+  </si>
+  <si>
+    <t>Adivina Cuánto te Quiero T01 EP12 HD</t>
+  </si>
+  <si>
+    <t>EEGHML112.ts</t>
+  </si>
+  <si>
+    <t>EEGHML113_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEGH7000000000000113</t>
+  </si>
+  <si>
+    <t>Adivina Cuánto te Quiero T01 EP13 HD</t>
+  </si>
+  <si>
+    <t>EEGHML113.ts</t>
+  </si>
+  <si>
+    <t>EEGHML114_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEGH7000000000000114</t>
+  </si>
+  <si>
+    <t>Adivina Cuánto te Quiero T01 EP14 HD</t>
+  </si>
+  <si>
+    <t>EEGHML114.ts</t>
+  </si>
+  <si>
+    <t>EEGHML115_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEGH7000000000000115</t>
+  </si>
+  <si>
+    <t>Adivina Cuánto te Quiero T01 EP15 HD</t>
+  </si>
+  <si>
+    <t>EEGHML115.ts</t>
+  </si>
+  <si>
+    <t>EEGHML116_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEGH7000000000000116</t>
+  </si>
+  <si>
+    <t>Adivina Cuánto te Quiero T01 EP16 HD</t>
+  </si>
+  <si>
+    <t>EEGHML116.ts</t>
+  </si>
+  <si>
+    <t>EEGHML117_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEGH7000000000000117</t>
+  </si>
+  <si>
+    <t>Adivina Cuánto te Quiero T01 EP17 HD</t>
+  </si>
+  <si>
+    <t>EEGHML117.ts</t>
+  </si>
+  <si>
+    <t>EEGHML118_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEGH7000000000000118</t>
+  </si>
+  <si>
+    <t>Adivina Cuánto te Quiero T01 EP18 HD</t>
+  </si>
+  <si>
+    <t>EEGHML118.ts</t>
+  </si>
+  <si>
+    <t>EEGHML119_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEGH7000000000000119</t>
+  </si>
+  <si>
+    <t>Adivina Cuánto te Quiero T01 EP19 HD</t>
+  </si>
+  <si>
+    <t>EEGHML119.ts</t>
+  </si>
+  <si>
+    <t>EEGHML120_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEGH7000000000000120</t>
+  </si>
+  <si>
+    <t>Adivina Cuánto te Quiero T01 EP20 HD</t>
+  </si>
+  <si>
+    <t>EEGHML120.ts</t>
+  </si>
+  <si>
+    <t>EEGHML121_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEGH7000000000000121</t>
+  </si>
+  <si>
+    <t>Adivina Cuánto te Quiero T01 EP21 HD</t>
+  </si>
+  <si>
+    <t>EEGHML121.ts</t>
+  </si>
+  <si>
+    <t>EEGHML122_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEGH7000000000000122</t>
+  </si>
+  <si>
+    <t>Adivina Cuánto te Quiero T01 EP22 HD</t>
+  </si>
+  <si>
+    <t>EEGHML122.ts</t>
+  </si>
+  <si>
+    <t>EEGHML123_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEGH7000000000000123</t>
+  </si>
+  <si>
+    <t>Adivina Cuánto te Quiero T01 EP23 HD</t>
+  </si>
+  <si>
+    <t>EEGHML123.ts</t>
+  </si>
+  <si>
+    <t>EEGHML124_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEGH7000000000000124</t>
+  </si>
+  <si>
+    <t>Adivina Cuánto te Quiero T01 EP24 HD</t>
+  </si>
+  <si>
+    <t>EEGHML124.ts</t>
+  </si>
+  <si>
+    <t>EEGHML125_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEGH7000000000000125</t>
+  </si>
+  <si>
+    <t>Adivina Cuánto te Quiero T01 EP25 HD</t>
+  </si>
+  <si>
+    <t>EEGHML125.ts</t>
+  </si>
+  <si>
+    <t>EEGHML126_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEGH7000000000000126</t>
+  </si>
+  <si>
+    <t>Adivina Cuánto te Quiero T01 EP26 HD</t>
+  </si>
+  <si>
+    <t>EEGHML126.ts</t>
   </si>
 </sst>
 </file>
@@ -1124,7 +1358,7 @@
   <dimension ref="A1:BF27"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:BF11"/>
+      <selection activeCell="A2" sqref="A2:BF17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1400,10 +1634,10 @@
         <v>48</v>
       </c>
       <c r="T2" s="10">
-        <v>7.9976851851851893E-3</v>
+        <v>7.5231481481481477E-3</v>
       </c>
       <c r="U2" s="11">
-        <v>8.3333333333333332E-3</v>
+        <v>7.6388888888888886E-3</v>
       </c>
       <c r="V2" s="3">
         <v>2012</v>
@@ -1418,7 +1652,7 @@
         <v>44</v>
       </c>
       <c r="Z2" s="4">
-        <v>43678</v>
+        <v>44409</v>
       </c>
       <c r="AA2" s="4">
         <v>45138</v>
@@ -1473,7 +1707,7 @@
         <v>56</v>
       </c>
       <c r="AS2" s="15">
-        <v>324551356</v>
+        <v>305322152</v>
       </c>
       <c r="AT2" s="9" t="s">
         <v>57</v>
@@ -1568,10 +1802,10 @@
         <v>48</v>
       </c>
       <c r="T3" s="10">
-        <v>7.9976851851851893E-3</v>
+        <v>7.5231481481481477E-3</v>
       </c>
       <c r="U3" s="11">
-        <v>8.3333333333333332E-3</v>
+        <v>7.6388888888888886E-3</v>
       </c>
       <c r="V3" s="3">
         <v>2012</v>
@@ -1586,7 +1820,7 @@
         <v>44</v>
       </c>
       <c r="Z3" s="4">
-        <v>43678</v>
+        <v>44409</v>
       </c>
       <c r="AA3" s="4">
         <v>45138</v>
@@ -1641,7 +1875,7 @@
         <v>56</v>
       </c>
       <c r="AS3" s="15">
-        <v>324551356</v>
+        <v>305350728</v>
       </c>
       <c r="AT3" s="9" t="s">
         <v>57</v>
@@ -1736,10 +1970,10 @@
         <v>48</v>
       </c>
       <c r="T4" s="10">
-        <v>7.9976851851851893E-3</v>
+        <v>7.5231481481481477E-3</v>
       </c>
       <c r="U4" s="11">
-        <v>8.3333333333333332E-3</v>
+        <v>7.6388888888888886E-3</v>
       </c>
       <c r="V4" s="3">
         <v>2012</v>
@@ -1754,7 +1988,7 @@
         <v>44</v>
       </c>
       <c r="Z4" s="4">
-        <v>43678</v>
+        <v>44409</v>
       </c>
       <c r="AA4" s="4">
         <v>45138</v>
@@ -1809,7 +2043,7 @@
         <v>56</v>
       </c>
       <c r="AS4" s="15">
-        <v>324491196</v>
+        <v>305350728</v>
       </c>
       <c r="AT4" s="9" t="s">
         <v>57</v>
@@ -1904,10 +2138,10 @@
         <v>48</v>
       </c>
       <c r="T5" s="10">
-        <v>7.9976851851851893E-3</v>
+        <v>7.5231481481481477E-3</v>
       </c>
       <c r="U5" s="11">
-        <v>8.3333333333333332E-3</v>
+        <v>7.6388888888888886E-3</v>
       </c>
       <c r="V5" s="3">
         <v>2012</v>
@@ -1922,7 +2156,7 @@
         <v>44</v>
       </c>
       <c r="Z5" s="4">
-        <v>43678</v>
+        <v>44409</v>
       </c>
       <c r="AA5" s="4">
         <v>45138</v>
@@ -1977,7 +2211,7 @@
         <v>56</v>
       </c>
       <c r="AS5" s="15">
-        <v>324508304</v>
+        <v>305350728</v>
       </c>
       <c r="AT5" s="9" t="s">
         <v>57</v>
@@ -2072,10 +2306,10 @@
         <v>48</v>
       </c>
       <c r="T6" s="10">
-        <v>7.9976851851851893E-3</v>
+        <v>7.5231481481481477E-3</v>
       </c>
       <c r="U6" s="11">
-        <v>8.3333333333333332E-3</v>
+        <v>7.6388888888888886E-3</v>
       </c>
       <c r="V6" s="3">
         <v>2012</v>
@@ -2090,7 +2324,7 @@
         <v>44</v>
       </c>
       <c r="Z6" s="4">
-        <v>43678</v>
+        <v>44409</v>
       </c>
       <c r="AA6" s="4">
         <v>45138</v>
@@ -2145,7 +2379,7 @@
         <v>56</v>
       </c>
       <c r="AS6" s="15">
-        <v>324508304</v>
+        <v>305350728</v>
       </c>
       <c r="AT6" s="9" t="s">
         <v>57</v>
@@ -2240,10 +2474,10 @@
         <v>48</v>
       </c>
       <c r="T7" s="10">
-        <v>7.9976851851851893E-3</v>
+        <v>7.5231481481481477E-3</v>
       </c>
       <c r="U7" s="11">
-        <v>8.3333333333333332E-3</v>
+        <v>7.6388888888888886E-3</v>
       </c>
       <c r="V7" s="3">
         <v>2012</v>
@@ -2258,7 +2492,7 @@
         <v>44</v>
       </c>
       <c r="Z7" s="4">
-        <v>43678</v>
+        <v>44409</v>
       </c>
       <c r="AA7" s="4">
         <v>45138</v>
@@ -2313,7 +2547,7 @@
         <v>56</v>
       </c>
       <c r="AS7" s="15">
-        <v>324508304</v>
+        <v>305350728</v>
       </c>
       <c r="AT7" s="9" t="s">
         <v>57</v>
@@ -2408,10 +2642,10 @@
         <v>48</v>
       </c>
       <c r="T8" s="10">
-        <v>7.9976851851851893E-3</v>
+        <v>7.5231481481481477E-3</v>
       </c>
       <c r="U8" s="11">
-        <v>8.3333333333333332E-3</v>
+        <v>7.6388888888888886E-3</v>
       </c>
       <c r="V8" s="3">
         <v>2012</v>
@@ -2426,7 +2660,7 @@
         <v>44</v>
       </c>
       <c r="Z8" s="4">
-        <v>43678</v>
+        <v>44409</v>
       </c>
       <c r="AA8" s="4">
         <v>45138</v>
@@ -2481,7 +2715,7 @@
         <v>56</v>
       </c>
       <c r="AS8" s="15">
-        <v>324491196</v>
+        <v>305350728</v>
       </c>
       <c r="AT8" s="9" t="s">
         <v>57</v>
@@ -2576,10 +2810,10 @@
         <v>48</v>
       </c>
       <c r="T9" s="10">
-        <v>7.9976851851851893E-3</v>
+        <v>7.5231481481481477E-3</v>
       </c>
       <c r="U9" s="11">
-        <v>8.3333333333333332E-3</v>
+        <v>7.6388888888888886E-3</v>
       </c>
       <c r="V9" s="3">
         <v>2012</v>
@@ -2594,7 +2828,7 @@
         <v>44</v>
       </c>
       <c r="Z9" s="4">
-        <v>43678</v>
+        <v>44409</v>
       </c>
       <c r="AA9" s="4">
         <v>45138</v>
@@ -2649,7 +2883,7 @@
         <v>56</v>
       </c>
       <c r="AS9" s="15">
-        <v>324491196</v>
+        <v>305350728</v>
       </c>
       <c r="AT9" s="9" t="s">
         <v>57</v>
@@ -2744,10 +2978,10 @@
         <v>48</v>
       </c>
       <c r="T10" s="10">
-        <v>7.9976851851851893E-3</v>
+        <v>7.5231481481481477E-3</v>
       </c>
       <c r="U10" s="11">
-        <v>8.3333333333333332E-3</v>
+        <v>7.6388888888888886E-3</v>
       </c>
       <c r="V10" s="3">
         <v>2012</v>
@@ -2762,7 +2996,7 @@
         <v>44</v>
       </c>
       <c r="Z10" s="4">
-        <v>43678</v>
+        <v>44409</v>
       </c>
       <c r="AA10" s="4">
         <v>45138</v>
@@ -2817,7 +3051,7 @@
         <v>56</v>
       </c>
       <c r="AS10" s="15">
-        <v>324491196</v>
+        <v>305350728</v>
       </c>
       <c r="AT10" s="9" t="s">
         <v>57</v>
@@ -2912,10 +3146,10 @@
         <v>48</v>
       </c>
       <c r="T11" s="10">
-        <v>7.9976851851851893E-3</v>
+        <v>7.5231481481481477E-3</v>
       </c>
       <c r="U11" s="11">
-        <v>8.3333333333333332E-3</v>
+        <v>7.6388888888888886E-3</v>
       </c>
       <c r="V11" s="3">
         <v>2012</v>
@@ -2930,7 +3164,7 @@
         <v>44</v>
       </c>
       <c r="Z11" s="4">
-        <v>43678</v>
+        <v>44409</v>
       </c>
       <c r="AA11" s="4">
         <v>45138</v>
@@ -2985,7 +3219,7 @@
         <v>56</v>
       </c>
       <c r="AS11" s="15">
-        <v>324508304</v>
+        <v>305350728</v>
       </c>
       <c r="AT11" s="9" t="s">
         <v>57</v>
@@ -3024,364 +3258,1012 @@
       </c>
     </row>
     <row r="12" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
+      <c r="A12" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="B12" s="7">
+        <v>44623</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="9">
+        <v>1</v>
+      </c>
+      <c r="G12" s="9">
+        <v>1</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>166</v>
+      </c>
       <c r="L12" s="8"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="9"/>
-      <c r="Q12" s="9"/>
-      <c r="R12" s="9"/>
-      <c r="S12" s="9"/>
-      <c r="T12" s="10"/>
-      <c r="U12" s="11"/>
-      <c r="V12" s="3"/>
-      <c r="W12" s="9"/>
-      <c r="X12" s="9"/>
-      <c r="Y12" s="9"/>
-      <c r="Z12" s="4"/>
-      <c r="AA12" s="4"/>
-      <c r="AB12" s="9"/>
-      <c r="AC12" s="9"/>
-      <c r="AD12" s="9"/>
-      <c r="AE12" s="9"/>
-      <c r="AF12" s="9"/>
-      <c r="AG12" s="9"/>
-      <c r="AH12" s="9"/>
-      <c r="AI12" s="9"/>
-      <c r="AJ12" s="9"/>
-      <c r="AK12" s="9"/>
+      <c r="M12" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="N12" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="O12" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="P12" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q12" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="R12" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="S12" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="T12" s="10">
+        <v>7.5231481481481477E-3</v>
+      </c>
+      <c r="U12" s="11">
+        <v>7.6388888888888886E-3</v>
+      </c>
+      <c r="V12" s="3">
+        <v>2012</v>
+      </c>
+      <c r="W12" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="X12" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y12" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z12" s="4">
+        <v>44409</v>
+      </c>
+      <c r="AA12" s="4">
+        <v>45138</v>
+      </c>
+      <c r="AB12" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC12" s="9">
+        <v>31028</v>
+      </c>
+      <c r="AD12" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE12" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF12" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="AG12" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="AH12" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI12" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="AJ12" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK12" s="9" t="s">
+        <v>88</v>
+      </c>
       <c r="AL12" s="8"/>
-      <c r="AM12" s="9"/>
-      <c r="AN12" s="9"/>
-      <c r="AO12" s="9"/>
-      <c r="AP12" s="9"/>
-      <c r="AQ12" s="9"/>
-      <c r="AR12" s="9"/>
-      <c r="AS12" s="9"/>
-      <c r="AT12" s="9"/>
-      <c r="AU12" s="9"/>
-      <c r="AV12" s="9"/>
+      <c r="AM12" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="AN12" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="AO12" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="AP12" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ12" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="AR12" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="AS12" s="9">
+        <v>305350728</v>
+      </c>
+      <c r="AT12" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="AU12" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="AV12" s="9" t="s">
+        <v>171</v>
+      </c>
       <c r="AW12" s="8"/>
-      <c r="AX12" s="9"/>
-      <c r="AY12" s="9"/>
-      <c r="AZ12" s="9"/>
+      <c r="AX12" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AY12" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AZ12" s="9" t="s">
+        <v>90</v>
+      </c>
       <c r="BA12" s="8"/>
-      <c r="BB12" s="9"/>
-      <c r="BC12" s="9"/>
-      <c r="BD12" s="9"/>
-      <c r="BE12" s="9"/>
-      <c r="BF12" s="9"/>
+      <c r="BB12" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="BC12" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="BD12" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="BE12" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="BF12" s="9" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="13" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
+      <c r="A13" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="B13" s="7">
+        <v>44623</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="9">
+        <v>1</v>
+      </c>
+      <c r="G13" s="9">
+        <v>1</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>175</v>
+      </c>
       <c r="L13" s="8"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="9"/>
-      <c r="Q13" s="9"/>
-      <c r="R13" s="9"/>
-      <c r="S13" s="9"/>
-      <c r="T13" s="10"/>
-      <c r="U13" s="11"/>
-      <c r="V13" s="3"/>
-      <c r="W13" s="9"/>
-      <c r="X13" s="9"/>
-      <c r="Y13" s="9"/>
-      <c r="Z13" s="4"/>
-      <c r="AA13" s="4"/>
-      <c r="AB13" s="9"/>
-      <c r="AC13" s="9"/>
-      <c r="AD13" s="9"/>
-      <c r="AE13" s="9"/>
-      <c r="AF13" s="9"/>
-      <c r="AG13" s="9"/>
-      <c r="AH13" s="9"/>
-      <c r="AI13" s="9"/>
-      <c r="AJ13" s="9"/>
-      <c r="AK13" s="9"/>
+      <c r="M13" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="N13" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="O13" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="P13" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q13" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="R13" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="S13" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="T13" s="10">
+        <v>7.5231481481481477E-3</v>
+      </c>
+      <c r="U13" s="11">
+        <v>7.6388888888888886E-3</v>
+      </c>
+      <c r="V13" s="3">
+        <v>2012</v>
+      </c>
+      <c r="W13" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="X13" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y13" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z13" s="4">
+        <v>44409</v>
+      </c>
+      <c r="AA13" s="4">
+        <v>45138</v>
+      </c>
+      <c r="AB13" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC13" s="9">
+        <v>31028</v>
+      </c>
+      <c r="AD13" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE13" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF13" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="AG13" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="AH13" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI13" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="AJ13" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK13" s="9" t="s">
+        <v>88</v>
+      </c>
       <c r="AL13" s="8"/>
-      <c r="AM13" s="9"/>
-      <c r="AN13" s="9"/>
-      <c r="AO13" s="9"/>
-      <c r="AP13" s="9"/>
-      <c r="AQ13" s="9"/>
-      <c r="AR13" s="9"/>
-      <c r="AS13" s="9"/>
-      <c r="AT13" s="9"/>
-      <c r="AU13" s="9"/>
-      <c r="AV13" s="9"/>
+      <c r="AM13" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="AN13" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="AO13" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="AP13" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ13" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="AR13" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="AS13" s="9">
+        <v>305350728</v>
+      </c>
+      <c r="AT13" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="AU13" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="AV13" s="9" t="s">
+        <v>180</v>
+      </c>
       <c r="AW13" s="8"/>
-      <c r="AX13" s="9"/>
-      <c r="AY13" s="9"/>
-      <c r="AZ13" s="9"/>
+      <c r="AX13" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AY13" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AZ13" s="9" t="s">
+        <v>90</v>
+      </c>
       <c r="BA13" s="8"/>
-      <c r="BB13" s="9"/>
-      <c r="BC13" s="9"/>
-      <c r="BD13" s="9"/>
-      <c r="BE13" s="9"/>
-      <c r="BF13" s="9"/>
+      <c r="BB13" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="BC13" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="BD13" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="BE13" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="BF13" s="9" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="14" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
+      <c r="A14" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="B14" s="7">
+        <v>44623</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" s="9">
+        <v>1</v>
+      </c>
+      <c r="G14" s="9">
+        <v>1</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>184</v>
+      </c>
       <c r="L14" s="8"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="9"/>
-      <c r="Q14" s="9"/>
-      <c r="R14" s="9"/>
-      <c r="S14" s="9"/>
-      <c r="T14" s="10"/>
-      <c r="U14" s="11"/>
-      <c r="V14" s="3"/>
-      <c r="W14" s="9"/>
-      <c r="X14" s="9"/>
-      <c r="Y14" s="9"/>
-      <c r="Z14" s="4"/>
-      <c r="AA14" s="4"/>
-      <c r="AB14" s="9"/>
-      <c r="AC14" s="9"/>
-      <c r="AD14" s="9"/>
-      <c r="AE14" s="9"/>
-      <c r="AF14" s="9"/>
-      <c r="AG14" s="9"/>
-      <c r="AH14" s="9"/>
-      <c r="AI14" s="9"/>
-      <c r="AJ14" s="9"/>
-      <c r="AK14" s="9"/>
+      <c r="M14" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="N14" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="O14" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="P14" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q14" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="R14" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="S14" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="T14" s="10">
+        <v>7.5231481481481477E-3</v>
+      </c>
+      <c r="U14" s="11">
+        <v>7.6388888888888886E-3</v>
+      </c>
+      <c r="V14" s="3">
+        <v>2012</v>
+      </c>
+      <c r="W14" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="X14" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y14" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z14" s="4">
+        <v>44409</v>
+      </c>
+      <c r="AA14" s="4">
+        <v>45138</v>
+      </c>
+      <c r="AB14" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC14" s="9">
+        <v>31028</v>
+      </c>
+      <c r="AD14" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE14" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF14" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="AG14" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="AH14" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI14" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="AJ14" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK14" s="9" t="s">
+        <v>88</v>
+      </c>
       <c r="AL14" s="8"/>
-      <c r="AM14" s="9"/>
-      <c r="AN14" s="9"/>
-      <c r="AO14" s="9"/>
-      <c r="AP14" s="9"/>
-      <c r="AQ14" s="9"/>
-      <c r="AR14" s="9"/>
-      <c r="AS14" s="9"/>
-      <c r="AT14" s="9"/>
-      <c r="AU14" s="9"/>
-      <c r="AV14" s="9"/>
+      <c r="AM14" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="AN14" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="AO14" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="AP14" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ14" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="AR14" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="AS14" s="9">
+        <v>305350728</v>
+      </c>
+      <c r="AT14" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="AU14" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="AV14" s="9" t="s">
+        <v>189</v>
+      </c>
       <c r="AW14" s="8"/>
-      <c r="AX14" s="9"/>
-      <c r="AY14" s="9"/>
-      <c r="AZ14" s="9"/>
+      <c r="AX14" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AY14" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AZ14" s="9" t="s">
+        <v>90</v>
+      </c>
       <c r="BA14" s="8"/>
-      <c r="BB14" s="9"/>
-      <c r="BC14" s="9"/>
-      <c r="BD14" s="9"/>
-      <c r="BE14" s="9"/>
-      <c r="BF14" s="9"/>
+      <c r="BB14" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="BC14" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="BD14" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="BE14" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="BF14" s="9" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="15" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
+      <c r="A15" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="B15" s="7">
+        <v>44623</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" s="9">
+        <v>1</v>
+      </c>
+      <c r="G15" s="9">
+        <v>1</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="J15" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="K15" s="9" t="s">
+        <v>193</v>
+      </c>
       <c r="L15" s="8"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="9"/>
-      <c r="P15" s="9"/>
-      <c r="Q15" s="9"/>
-      <c r="R15" s="9"/>
-      <c r="S15" s="9"/>
-      <c r="T15" s="10"/>
-      <c r="U15" s="11"/>
-      <c r="V15" s="3"/>
-      <c r="W15" s="9"/>
-      <c r="X15" s="9"/>
-      <c r="Y15" s="9"/>
-      <c r="Z15" s="4"/>
-      <c r="AA15" s="4"/>
-      <c r="AB15" s="9"/>
-      <c r="AC15" s="9"/>
-      <c r="AD15" s="9"/>
-      <c r="AE15" s="9"/>
-      <c r="AF15" s="9"/>
-      <c r="AG15" s="9"/>
-      <c r="AH15" s="9"/>
-      <c r="AI15" s="9"/>
-      <c r="AJ15" s="9"/>
-      <c r="AK15" s="9"/>
+      <c r="M15" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="N15" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="O15" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="P15" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="Q15" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="R15" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="S15" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="T15" s="10">
+        <v>7.5231481481481477E-3</v>
+      </c>
+      <c r="U15" s="11">
+        <v>7.6388888888888886E-3</v>
+      </c>
+      <c r="V15" s="3">
+        <v>2012</v>
+      </c>
+      <c r="W15" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="X15" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y15" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z15" s="4">
+        <v>44409</v>
+      </c>
+      <c r="AA15" s="4">
+        <v>45138</v>
+      </c>
+      <c r="AB15" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC15" s="9">
+        <v>31028</v>
+      </c>
+      <c r="AD15" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE15" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF15" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="AG15" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="AH15" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI15" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="AJ15" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK15" s="9" t="s">
+        <v>88</v>
+      </c>
       <c r="AL15" s="8"/>
-      <c r="AM15" s="9"/>
-      <c r="AN15" s="9"/>
-      <c r="AO15" s="9"/>
-      <c r="AP15" s="9"/>
-      <c r="AQ15" s="9"/>
-      <c r="AR15" s="9"/>
-      <c r="AS15" s="9"/>
-      <c r="AT15" s="9"/>
-      <c r="AU15" s="9"/>
-      <c r="AV15" s="9"/>
+      <c r="AM15" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="AN15" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="AO15" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="AP15" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ15" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="AR15" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="AS15" s="9">
+        <v>305350728</v>
+      </c>
+      <c r="AT15" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="AU15" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="AV15" s="9" t="s">
+        <v>198</v>
+      </c>
       <c r="AW15" s="8"/>
-      <c r="AX15" s="9"/>
-      <c r="AY15" s="9"/>
-      <c r="AZ15" s="9"/>
+      <c r="AX15" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AY15" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AZ15" s="9" t="s">
+        <v>90</v>
+      </c>
       <c r="BA15" s="8"/>
-      <c r="BB15" s="9"/>
-      <c r="BC15" s="9"/>
-      <c r="BD15" s="9"/>
-      <c r="BE15" s="9"/>
-      <c r="BF15" s="9"/>
+      <c r="BB15" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="BC15" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="BD15" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="BE15" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="BF15" s="9" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="16" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
+      <c r="A16" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="B16" s="7">
+        <v>44623</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="9">
+        <v>1</v>
+      </c>
+      <c r="G16" s="9">
+        <v>1</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="J16" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="K16" s="9" t="s">
+        <v>202</v>
+      </c>
       <c r="L16" s="8"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="9"/>
-      <c r="P16" s="9"/>
-      <c r="Q16" s="9"/>
-      <c r="R16" s="9"/>
-      <c r="S16" s="9"/>
-      <c r="T16" s="10"/>
-      <c r="U16" s="11"/>
-      <c r="V16" s="3"/>
-      <c r="W16" s="9"/>
-      <c r="X16" s="9"/>
-      <c r="Y16" s="9"/>
-      <c r="Z16" s="4"/>
-      <c r="AA16" s="4"/>
-      <c r="AB16" s="9"/>
-      <c r="AC16" s="9"/>
-      <c r="AD16" s="9"/>
-      <c r="AE16" s="9"/>
-      <c r="AF16" s="9"/>
-      <c r="AG16" s="9"/>
-      <c r="AH16" s="9"/>
-      <c r="AI16" s="9"/>
-      <c r="AJ16" s="9"/>
-      <c r="AK16" s="9"/>
+      <c r="M16" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="N16" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="O16" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="P16" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="Q16" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="R16" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="S16" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="T16" s="10">
+        <v>7.5231481481481477E-3</v>
+      </c>
+      <c r="U16" s="11">
+        <v>7.6388888888888886E-3</v>
+      </c>
+      <c r="V16" s="3">
+        <v>2012</v>
+      </c>
+      <c r="W16" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="X16" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y16" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z16" s="4">
+        <v>44409</v>
+      </c>
+      <c r="AA16" s="4">
+        <v>45138</v>
+      </c>
+      <c r="AB16" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC16" s="9">
+        <v>31028</v>
+      </c>
+      <c r="AD16" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE16" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF16" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="AG16" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="AH16" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI16" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="AJ16" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK16" s="9" t="s">
+        <v>88</v>
+      </c>
       <c r="AL16" s="8"/>
-      <c r="AM16" s="9"/>
-      <c r="AN16" s="9"/>
-      <c r="AO16" s="9"/>
-      <c r="AP16" s="9"/>
-      <c r="AQ16" s="9"/>
-      <c r="AR16" s="9"/>
-      <c r="AS16" s="9"/>
-      <c r="AT16" s="9"/>
-      <c r="AU16" s="9"/>
-      <c r="AV16" s="9"/>
+      <c r="AM16" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="AN16" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="AO16" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="AP16" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ16" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="AR16" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="AS16" s="9">
+        <v>305350728</v>
+      </c>
+      <c r="AT16" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="AU16" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="AV16" s="9" t="s">
+        <v>207</v>
+      </c>
       <c r="AW16" s="8"/>
-      <c r="AX16" s="9"/>
-      <c r="AY16" s="9"/>
-      <c r="AZ16" s="9"/>
+      <c r="AX16" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AY16" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AZ16" s="9" t="s">
+        <v>90</v>
+      </c>
       <c r="BA16" s="8"/>
-      <c r="BB16" s="9"/>
-      <c r="BC16" s="9"/>
-      <c r="BD16" s="9"/>
-      <c r="BE16" s="9"/>
-      <c r="BF16" s="9"/>
+      <c r="BB16" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="BC16" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="BD16" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="BE16" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="BF16" s="9" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="17" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
+      <c r="A17" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="B17" s="7">
+        <v>44623</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" s="9">
+        <v>1</v>
+      </c>
+      <c r="G17" s="9">
+        <v>1</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J17" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="K17" s="9" t="s">
+        <v>211</v>
+      </c>
       <c r="L17" s="8"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="9"/>
-      <c r="P17" s="9"/>
-      <c r="Q17" s="9"/>
-      <c r="R17" s="9"/>
-      <c r="S17" s="9"/>
-      <c r="T17" s="10"/>
-      <c r="U17" s="11"/>
-      <c r="V17" s="3"/>
-      <c r="W17" s="9"/>
-      <c r="X17" s="9"/>
-      <c r="Y17" s="9"/>
-      <c r="Z17" s="4"/>
-      <c r="AA17" s="4"/>
-      <c r="AB17" s="9"/>
-      <c r="AC17" s="9"/>
-      <c r="AD17" s="9"/>
-      <c r="AE17" s="9"/>
-      <c r="AF17" s="9"/>
-      <c r="AG17" s="9"/>
-      <c r="AH17" s="9"/>
-      <c r="AI17" s="9"/>
-      <c r="AJ17" s="9"/>
-      <c r="AK17" s="9"/>
+      <c r="M17" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="N17" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="O17" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="P17" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="Q17" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="R17" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="S17" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="T17" s="10">
+        <v>7.5231481481481477E-3</v>
+      </c>
+      <c r="U17" s="11">
+        <v>7.6388888888888886E-3</v>
+      </c>
+      <c r="V17" s="3">
+        <v>2012</v>
+      </c>
+      <c r="W17" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="X17" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y17" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z17" s="4">
+        <v>44409</v>
+      </c>
+      <c r="AA17" s="4">
+        <v>45138</v>
+      </c>
+      <c r="AB17" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC17" s="9">
+        <v>31028</v>
+      </c>
+      <c r="AD17" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE17" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF17" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="AG17" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="AH17" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI17" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="AJ17" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK17" s="9" t="s">
+        <v>88</v>
+      </c>
       <c r="AL17" s="8"/>
-      <c r="AM17" s="9"/>
-      <c r="AN17" s="9"/>
-      <c r="AO17" s="9"/>
-      <c r="AP17" s="9"/>
-      <c r="AQ17" s="9"/>
-      <c r="AR17" s="9"/>
-      <c r="AS17" s="9"/>
-      <c r="AT17" s="9"/>
-      <c r="AU17" s="9"/>
-      <c r="AV17" s="9"/>
+      <c r="AM17" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="AN17" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="AO17" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="AP17" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ17" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="AR17" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="AS17" s="9">
+        <v>305350728</v>
+      </c>
+      <c r="AT17" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="AU17" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="AV17" s="9" t="s">
+        <v>216</v>
+      </c>
       <c r="AW17" s="8"/>
-      <c r="AX17" s="9"/>
-      <c r="AY17" s="9"/>
-      <c r="AZ17" s="9"/>
+      <c r="AX17" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AY17" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AZ17" s="9" t="s">
+        <v>90</v>
+      </c>
       <c r="BA17" s="8"/>
-      <c r="BB17" s="9"/>
-      <c r="BC17" s="9"/>
-      <c r="BD17" s="9"/>
-      <c r="BE17" s="9"/>
-      <c r="BF17" s="9"/>
+      <c r="BB17" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="BC17" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="BD17" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="BE17" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="BF17" s="9" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="18" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
@@ -3993,7 +4875,7 @@
   <dimension ref="A1:BF25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:BF11"/>
+      <selection activeCell="A2" sqref="A2:BF17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4213,7 +5095,7 @@
     </row>
     <row r="2" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>164</v>
+        <v>218</v>
       </c>
       <c r="B2" s="12">
         <v>44623</v>
@@ -4237,7 +5119,7 @@
         <v>46</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>165</v>
+        <v>219</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>78</v>
@@ -4253,7 +5135,7 @@
         <v>47</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>166</v>
+        <v>220</v>
       </c>
       <c r="P2" s="9" t="s">
         <v>66</v>
@@ -4268,10 +5150,10 @@
         <v>48</v>
       </c>
       <c r="T2" s="10">
-        <v>7.9976851851851893E-3</v>
+        <v>7.5231481481481477E-3</v>
       </c>
       <c r="U2" s="11">
-        <v>8.3333333333333332E-3</v>
+        <v>7.6388888888888886E-3</v>
       </c>
       <c r="V2" s="9">
         <v>2012</v>
@@ -4286,7 +5168,7 @@
         <v>44</v>
       </c>
       <c r="Z2" s="4">
-        <v>43678</v>
+        <v>44409</v>
       </c>
       <c r="AA2" s="4">
         <v>45138</v>
@@ -4341,7 +5223,7 @@
         <v>56</v>
       </c>
       <c r="AS2" s="15">
-        <v>649045184</v>
+        <v>610586588</v>
       </c>
       <c r="AT2" s="9" t="s">
         <v>56</v>
@@ -4350,7 +5232,7 @@
         <v>63</v>
       </c>
       <c r="AV2" s="9" t="s">
-        <v>167</v>
+        <v>221</v>
       </c>
       <c r="AW2" s="8"/>
       <c r="AX2" s="9" t="s">
@@ -4381,7 +5263,7 @@
     </row>
     <row r="3" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>168</v>
+        <v>222</v>
       </c>
       <c r="B3" s="12">
         <v>44623</v>
@@ -4405,7 +5287,7 @@
         <v>46</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>169</v>
+        <v>223</v>
       </c>
       <c r="J3" s="9" t="s">
         <v>78</v>
@@ -4421,7 +5303,7 @@
         <v>47</v>
       </c>
       <c r="O3" s="9" t="s">
-        <v>170</v>
+        <v>224</v>
       </c>
       <c r="P3" s="9" t="s">
         <v>67</v>
@@ -4436,10 +5318,10 @@
         <v>48</v>
       </c>
       <c r="T3" s="10">
-        <v>7.9976851851851893E-3</v>
+        <v>7.5231481481481477E-3</v>
       </c>
       <c r="U3" s="11">
-        <v>8.3333333333333332E-3</v>
+        <v>7.6388888888888886E-3</v>
       </c>
       <c r="V3" s="9">
         <v>2012</v>
@@ -4454,7 +5336,7 @@
         <v>44</v>
       </c>
       <c r="Z3" s="4">
-        <v>43678</v>
+        <v>44409</v>
       </c>
       <c r="AA3" s="4">
         <v>45138</v>
@@ -4509,7 +5391,7 @@
         <v>56</v>
       </c>
       <c r="AS3" s="15">
-        <v>649045184</v>
+        <v>610643928</v>
       </c>
       <c r="AT3" s="9" t="s">
         <v>56</v>
@@ -4518,7 +5400,7 @@
         <v>63</v>
       </c>
       <c r="AV3" s="9" t="s">
-        <v>171</v>
+        <v>225</v>
       </c>
       <c r="AW3" s="8"/>
       <c r="AX3" s="9" t="s">
@@ -4549,7 +5431,7 @@
     </row>
     <row r="4" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>172</v>
+        <v>226</v>
       </c>
       <c r="B4" s="12">
         <v>44623</v>
@@ -4573,7 +5455,7 @@
         <v>46</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>173</v>
+        <v>227</v>
       </c>
       <c r="J4" s="9" t="s">
         <v>78</v>
@@ -4589,7 +5471,7 @@
         <v>47</v>
       </c>
       <c r="O4" s="9" t="s">
-        <v>174</v>
+        <v>228</v>
       </c>
       <c r="P4" s="9" t="s">
         <v>68</v>
@@ -4604,10 +5486,10 @@
         <v>48</v>
       </c>
       <c r="T4" s="10">
-        <v>7.9976851851851893E-3</v>
+        <v>7.5231481481481477E-3</v>
       </c>
       <c r="U4" s="11">
-        <v>8.3333333333333332E-3</v>
+        <v>7.6388888888888886E-3</v>
       </c>
       <c r="V4" s="9">
         <v>2012</v>
@@ -4622,7 +5504,7 @@
         <v>44</v>
       </c>
       <c r="Z4" s="4">
-        <v>43678</v>
+        <v>44409</v>
       </c>
       <c r="AA4" s="4">
         <v>45138</v>
@@ -4677,7 +5559,7 @@
         <v>56</v>
       </c>
       <c r="AS4" s="15">
-        <v>648924676</v>
+        <v>610643928</v>
       </c>
       <c r="AT4" s="9" t="s">
         <v>56</v>
@@ -4686,7 +5568,7 @@
         <v>63</v>
       </c>
       <c r="AV4" s="9" t="s">
-        <v>175</v>
+        <v>229</v>
       </c>
       <c r="AW4" s="8"/>
       <c r="AX4" s="9" t="s">
@@ -4717,7 +5599,7 @@
     </row>
     <row r="5" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>176</v>
+        <v>230</v>
       </c>
       <c r="B5" s="12">
         <v>44623</v>
@@ -4741,7 +5623,7 @@
         <v>46</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>177</v>
+        <v>231</v>
       </c>
       <c r="J5" s="9" t="s">
         <v>78</v>
@@ -4757,7 +5639,7 @@
         <v>47</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>178</v>
+        <v>232</v>
       </c>
       <c r="P5" s="9" t="s">
         <v>69</v>
@@ -4772,10 +5654,10 @@
         <v>48</v>
       </c>
       <c r="T5" s="10">
-        <v>7.9976851851851893E-3</v>
+        <v>7.5231481481481477E-3</v>
       </c>
       <c r="U5" s="11">
-        <v>8.3333333333333332E-3</v>
+        <v>7.6388888888888886E-3</v>
       </c>
       <c r="V5" s="9">
         <v>2012</v>
@@ -4790,7 +5672,7 @@
         <v>44</v>
       </c>
       <c r="Z5" s="4">
-        <v>43678</v>
+        <v>44409</v>
       </c>
       <c r="AA5" s="4">
         <v>45138</v>
@@ -4845,7 +5727,7 @@
         <v>56</v>
       </c>
       <c r="AS5" s="15">
-        <v>648924676</v>
+        <v>610643928</v>
       </c>
       <c r="AT5" s="9" t="s">
         <v>56</v>
@@ -4854,7 +5736,7 @@
         <v>63</v>
       </c>
       <c r="AV5" s="9" t="s">
-        <v>179</v>
+        <v>233</v>
       </c>
       <c r="AW5" s="8"/>
       <c r="AX5" s="9" t="s">
@@ -4885,7 +5767,7 @@
     </row>
     <row r="6" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>180</v>
+        <v>234</v>
       </c>
       <c r="B6" s="12">
         <v>44623</v>
@@ -4909,7 +5791,7 @@
         <v>46</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>181</v>
+        <v>235</v>
       </c>
       <c r="J6" s="9" t="s">
         <v>78</v>
@@ -4925,7 +5807,7 @@
         <v>47</v>
       </c>
       <c r="O6" s="9" t="s">
-        <v>182</v>
+        <v>236</v>
       </c>
       <c r="P6" s="9" t="s">
         <v>70</v>
@@ -4940,10 +5822,10 @@
         <v>48</v>
       </c>
       <c r="T6" s="10">
-        <v>7.9976851851851893E-3</v>
+        <v>7.5231481481481477E-3</v>
       </c>
       <c r="U6" s="11">
-        <v>8.3333333333333332E-3</v>
+        <v>7.6388888888888886E-3</v>
       </c>
       <c r="V6" s="9">
         <v>2012</v>
@@ -4958,7 +5840,7 @@
         <v>44</v>
       </c>
       <c r="Z6" s="4">
-        <v>43678</v>
+        <v>44409</v>
       </c>
       <c r="AA6" s="4">
         <v>45138</v>
@@ -5013,7 +5895,7 @@
         <v>56</v>
       </c>
       <c r="AS6" s="15">
-        <v>648953440</v>
+        <v>610643928</v>
       </c>
       <c r="AT6" s="9" t="s">
         <v>56</v>
@@ -5022,7 +5904,7 @@
         <v>63</v>
       </c>
       <c r="AV6" s="9" t="s">
-        <v>183</v>
+        <v>237</v>
       </c>
       <c r="AW6" s="8"/>
       <c r="AX6" s="9" t="s">
@@ -5053,7 +5935,7 @@
     </row>
     <row r="7" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>184</v>
+        <v>238</v>
       </c>
       <c r="B7" s="12">
         <v>44623</v>
@@ -5077,7 +5959,7 @@
         <v>46</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>185</v>
+        <v>239</v>
       </c>
       <c r="J7" s="9" t="s">
         <v>78</v>
@@ -5093,7 +5975,7 @@
         <v>47</v>
       </c>
       <c r="O7" s="9" t="s">
-        <v>186</v>
+        <v>240</v>
       </c>
       <c r="P7" s="9" t="s">
         <v>71</v>
@@ -5108,10 +5990,10 @@
         <v>48</v>
       </c>
       <c r="T7" s="10">
-        <v>7.9976851851851893E-3</v>
+        <v>7.5231481481481477E-3</v>
       </c>
       <c r="U7" s="11">
-        <v>8.3333333333333332E-3</v>
+        <v>7.6388888888888886E-3</v>
       </c>
       <c r="V7" s="9">
         <v>2012</v>
@@ -5126,7 +6008,7 @@
         <v>44</v>
       </c>
       <c r="Z7" s="4">
-        <v>43678</v>
+        <v>44409</v>
       </c>
       <c r="AA7" s="4">
         <v>45138</v>
@@ -5181,7 +6063,7 @@
         <v>56</v>
       </c>
       <c r="AS7" s="15">
-        <v>648953440</v>
+        <v>610643928</v>
       </c>
       <c r="AT7" s="9" t="s">
         <v>56</v>
@@ -5190,7 +6072,7 @@
         <v>63</v>
       </c>
       <c r="AV7" s="9" t="s">
-        <v>187</v>
+        <v>241</v>
       </c>
       <c r="AW7" s="8"/>
       <c r="AX7" s="9" t="s">
@@ -5221,7 +6103,7 @@
     </row>
     <row r="8" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>188</v>
+        <v>242</v>
       </c>
       <c r="B8" s="12">
         <v>44623</v>
@@ -5245,7 +6127,7 @@
         <v>46</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>189</v>
+        <v>243</v>
       </c>
       <c r="J8" s="9" t="s">
         <v>78</v>
@@ -5261,7 +6143,7 @@
         <v>47</v>
       </c>
       <c r="O8" s="9" t="s">
-        <v>190</v>
+        <v>244</v>
       </c>
       <c r="P8" s="9" t="s">
         <v>72</v>
@@ -5276,10 +6158,10 @@
         <v>48</v>
       </c>
       <c r="T8" s="10">
-        <v>7.9976851851851893E-3</v>
+        <v>7.5231481481481477E-3</v>
       </c>
       <c r="U8" s="11">
-        <v>8.3333333333333332E-3</v>
+        <v>7.6388888888888886E-3</v>
       </c>
       <c r="V8" s="9">
         <v>2012</v>
@@ -5294,7 +6176,7 @@
         <v>44</v>
       </c>
       <c r="Z8" s="4">
-        <v>43678</v>
+        <v>44409</v>
       </c>
       <c r="AA8" s="4">
         <v>45138</v>
@@ -5349,7 +6231,7 @@
         <v>56</v>
       </c>
       <c r="AS8" s="15">
-        <v>648924676</v>
+        <v>610643928</v>
       </c>
       <c r="AT8" s="9" t="s">
         <v>56</v>
@@ -5358,7 +6240,7 @@
         <v>63</v>
       </c>
       <c r="AV8" s="9" t="s">
-        <v>191</v>
+        <v>245</v>
       </c>
       <c r="AW8" s="8"/>
       <c r="AX8" s="9" t="s">
@@ -5389,7 +6271,7 @@
     </row>
     <row r="9" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>192</v>
+        <v>246</v>
       </c>
       <c r="B9" s="12">
         <v>44623</v>
@@ -5413,7 +6295,7 @@
         <v>46</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>193</v>
+        <v>247</v>
       </c>
       <c r="J9" s="9" t="s">
         <v>78</v>
@@ -5429,7 +6311,7 @@
         <v>47</v>
       </c>
       <c r="O9" s="9" t="s">
-        <v>194</v>
+        <v>248</v>
       </c>
       <c r="P9" s="9" t="s">
         <v>73</v>
@@ -5444,10 +6326,10 @@
         <v>48</v>
       </c>
       <c r="T9" s="10">
-        <v>7.9976851851851893E-3</v>
+        <v>7.5231481481481477E-3</v>
       </c>
       <c r="U9" s="11">
-        <v>8.3333333333333332E-3</v>
+        <v>7.6388888888888886E-3</v>
       </c>
       <c r="V9" s="9">
         <v>2012</v>
@@ -5462,7 +6344,7 @@
         <v>44</v>
       </c>
       <c r="Z9" s="4">
-        <v>43678</v>
+        <v>44409</v>
       </c>
       <c r="AA9" s="4">
         <v>45138</v>
@@ -5517,7 +6399,7 @@
         <v>56</v>
       </c>
       <c r="AS9" s="15">
-        <v>648924676</v>
+        <v>610643928</v>
       </c>
       <c r="AT9" s="9" t="s">
         <v>56</v>
@@ -5526,7 +6408,7 @@
         <v>63</v>
       </c>
       <c r="AV9" s="9" t="s">
-        <v>195</v>
+        <v>249</v>
       </c>
       <c r="AW9" s="8"/>
       <c r="AX9" s="9" t="s">
@@ -5557,7 +6439,7 @@
     </row>
     <row r="10" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>196</v>
+        <v>250</v>
       </c>
       <c r="B10" s="12">
         <v>44623</v>
@@ -5581,7 +6463,7 @@
         <v>46</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>197</v>
+        <v>251</v>
       </c>
       <c r="J10" s="9" t="s">
         <v>78</v>
@@ -5597,7 +6479,7 @@
         <v>47</v>
       </c>
       <c r="O10" s="9" t="s">
-        <v>198</v>
+        <v>252</v>
       </c>
       <c r="P10" s="9" t="s">
         <v>74</v>
@@ -5612,10 +6494,10 @@
         <v>48</v>
       </c>
       <c r="T10" s="10">
-        <v>7.9976851851851893E-3</v>
+        <v>7.5231481481481477E-3</v>
       </c>
       <c r="U10" s="11">
-        <v>8.3333333333333332E-3</v>
+        <v>7.6388888888888886E-3</v>
       </c>
       <c r="V10" s="9">
         <v>2012</v>
@@ -5630,7 +6512,7 @@
         <v>44</v>
       </c>
       <c r="Z10" s="4">
-        <v>43678</v>
+        <v>44409</v>
       </c>
       <c r="AA10" s="4">
         <v>45138</v>
@@ -5685,7 +6567,7 @@
         <v>56</v>
       </c>
       <c r="AS10" s="15">
-        <v>648924676</v>
+        <v>610643928</v>
       </c>
       <c r="AT10" s="9" t="s">
         <v>56</v>
@@ -5694,7 +6576,7 @@
         <v>63</v>
       </c>
       <c r="AV10" s="9" t="s">
-        <v>199</v>
+        <v>253</v>
       </c>
       <c r="AW10" s="8"/>
       <c r="AX10" s="9" t="s">
@@ -5725,7 +6607,7 @@
     </row>
     <row r="11" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>200</v>
+        <v>254</v>
       </c>
       <c r="B11" s="12">
         <v>44623</v>
@@ -5749,7 +6631,7 @@
         <v>46</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>201</v>
+        <v>255</v>
       </c>
       <c r="J11" s="9" t="s">
         <v>78</v>
@@ -5765,7 +6647,7 @@
         <v>47</v>
       </c>
       <c r="O11" s="9" t="s">
-        <v>202</v>
+        <v>256</v>
       </c>
       <c r="P11" s="9" t="s">
         <v>75</v>
@@ -5780,10 +6662,10 @@
         <v>48</v>
       </c>
       <c r="T11" s="10">
-        <v>7.9976851851851893E-3</v>
+        <v>7.5231481481481477E-3</v>
       </c>
       <c r="U11" s="11">
-        <v>8.3333333333333332E-3</v>
+        <v>7.6388888888888886E-3</v>
       </c>
       <c r="V11" s="9">
         <v>2012</v>
@@ -5798,7 +6680,7 @@
         <v>44</v>
       </c>
       <c r="Z11" s="4">
-        <v>43678</v>
+        <v>44409</v>
       </c>
       <c r="AA11" s="4">
         <v>45138</v>
@@ -5853,7 +6735,7 @@
         <v>56</v>
       </c>
       <c r="AS11" s="9">
-        <v>648953440</v>
+        <v>610643928</v>
       </c>
       <c r="AT11" s="9" t="s">
         <v>56</v>
@@ -5862,7 +6744,7 @@
         <v>63</v>
       </c>
       <c r="AV11" s="9" t="s">
-        <v>203</v>
+        <v>257</v>
       </c>
       <c r="AW11" s="8"/>
       <c r="AX11" s="9" t="s">
@@ -5892,364 +6774,1012 @@
       </c>
     </row>
     <row r="12" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
+      <c r="A12" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="B12" s="12">
+        <v>44623</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="9">
+        <v>1</v>
+      </c>
+      <c r="G12" s="9">
+        <v>1</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>166</v>
+      </c>
       <c r="L12" s="8"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="9"/>
-      <c r="Q12" s="9"/>
-      <c r="R12" s="9"/>
-      <c r="S12" s="9"/>
-      <c r="T12" s="10"/>
-      <c r="U12" s="11"/>
-      <c r="V12" s="9"/>
-      <c r="W12" s="9"/>
-      <c r="X12" s="9"/>
-      <c r="Y12" s="9"/>
-      <c r="Z12" s="4"/>
-      <c r="AA12" s="4"/>
-      <c r="AB12" s="9"/>
-      <c r="AC12" s="9"/>
-      <c r="AD12" s="9"/>
-      <c r="AE12" s="9"/>
-      <c r="AF12" s="9"/>
-      <c r="AG12" s="9"/>
-      <c r="AH12" s="9"/>
-      <c r="AI12" s="9"/>
-      <c r="AJ12" s="9"/>
-      <c r="AK12" s="9"/>
+      <c r="M12" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="N12" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="O12" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="P12" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q12" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="R12" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="S12" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="T12" s="10">
+        <v>7.5231481481481477E-3</v>
+      </c>
+      <c r="U12" s="11">
+        <v>7.6388888888888886E-3</v>
+      </c>
+      <c r="V12" s="9">
+        <v>2012</v>
+      </c>
+      <c r="W12" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="X12" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y12" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z12" s="4">
+        <v>44409</v>
+      </c>
+      <c r="AA12" s="4">
+        <v>45138</v>
+      </c>
+      <c r="AB12" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC12" s="9">
+        <v>31028</v>
+      </c>
+      <c r="AD12" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE12" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF12" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="AG12" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="AH12" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI12" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="AJ12" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK12" s="9" t="s">
+        <v>88</v>
+      </c>
       <c r="AL12" s="8"/>
-      <c r="AM12" s="9"/>
-      <c r="AN12" s="9"/>
-      <c r="AO12" s="9"/>
-      <c r="AP12" s="9"/>
-      <c r="AQ12" s="9"/>
-      <c r="AR12" s="9"/>
-      <c r="AS12" s="9"/>
-      <c r="AT12" s="9"/>
-      <c r="AU12" s="9"/>
-      <c r="AV12" s="9"/>
+      <c r="AM12" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="AN12" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="AO12" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="AP12" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ12" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="AR12" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="AS12" s="9">
+        <v>610643928</v>
+      </c>
+      <c r="AT12" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="AU12" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="AV12" s="9" t="s">
+        <v>261</v>
+      </c>
       <c r="AW12" s="8"/>
-      <c r="AX12" s="9"/>
-      <c r="AY12" s="9"/>
-      <c r="AZ12" s="9"/>
+      <c r="AX12" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AY12" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AZ12" s="9" t="s">
+        <v>90</v>
+      </c>
       <c r="BA12" s="8"/>
-      <c r="BB12" s="9"/>
-      <c r="BC12" s="9"/>
-      <c r="BD12" s="9"/>
-      <c r="BE12" s="9"/>
-      <c r="BF12" s="9"/>
+      <c r="BB12" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="BC12" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="BD12" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="BE12" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="BF12" s="9" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="13" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
+      <c r="A13" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="B13" s="12">
+        <v>44623</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="9">
+        <v>1</v>
+      </c>
+      <c r="G13" s="9">
+        <v>1</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>175</v>
+      </c>
       <c r="L13" s="8"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="9"/>
-      <c r="Q13" s="9"/>
-      <c r="R13" s="9"/>
-      <c r="S13" s="9"/>
-      <c r="T13" s="10"/>
-      <c r="U13" s="11"/>
-      <c r="V13" s="9"/>
-      <c r="W13" s="9"/>
-      <c r="X13" s="9"/>
-      <c r="Y13" s="9"/>
-      <c r="Z13" s="4"/>
-      <c r="AA13" s="4"/>
-      <c r="AB13" s="9"/>
-      <c r="AC13" s="9"/>
-      <c r="AD13" s="9"/>
-      <c r="AE13" s="9"/>
-      <c r="AF13" s="9"/>
-      <c r="AG13" s="9"/>
-      <c r="AH13" s="9"/>
-      <c r="AI13" s="9"/>
-      <c r="AJ13" s="9"/>
-      <c r="AK13" s="9"/>
+      <c r="M13" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="N13" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="O13" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="P13" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q13" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="R13" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="S13" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="T13" s="10">
+        <v>7.5231481481481477E-3</v>
+      </c>
+      <c r="U13" s="11">
+        <v>7.6388888888888886E-3</v>
+      </c>
+      <c r="V13" s="9">
+        <v>2012</v>
+      </c>
+      <c r="W13" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="X13" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y13" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z13" s="4">
+        <v>44409</v>
+      </c>
+      <c r="AA13" s="4">
+        <v>45138</v>
+      </c>
+      <c r="AB13" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC13" s="9">
+        <v>31028</v>
+      </c>
+      <c r="AD13" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE13" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF13" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="AG13" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="AH13" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI13" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="AJ13" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK13" s="9" t="s">
+        <v>88</v>
+      </c>
       <c r="AL13" s="8"/>
-      <c r="AM13" s="9"/>
-      <c r="AN13" s="9"/>
-      <c r="AO13" s="9"/>
-      <c r="AP13" s="9"/>
-      <c r="AQ13" s="9"/>
-      <c r="AR13" s="9"/>
-      <c r="AS13" s="9"/>
-      <c r="AT13" s="9"/>
-      <c r="AU13" s="9"/>
-      <c r="AV13" s="9"/>
+      <c r="AM13" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="AN13" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="AO13" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="AP13" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ13" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="AR13" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="AS13" s="9">
+        <v>610643928</v>
+      </c>
+      <c r="AT13" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="AU13" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="AV13" s="9" t="s">
+        <v>265</v>
+      </c>
       <c r="AW13" s="8"/>
-      <c r="AX13" s="9"/>
-      <c r="AY13" s="9"/>
-      <c r="AZ13" s="9"/>
+      <c r="AX13" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AY13" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AZ13" s="9" t="s">
+        <v>90</v>
+      </c>
       <c r="BA13" s="8"/>
-      <c r="BB13" s="9"/>
-      <c r="BC13" s="9"/>
-      <c r="BD13" s="9"/>
-      <c r="BE13" s="9"/>
-      <c r="BF13" s="9"/>
+      <c r="BB13" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="BC13" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="BD13" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="BE13" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="BF13" s="9" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="14" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
+      <c r="A14" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="B14" s="12">
+        <v>44623</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" s="9">
+        <v>1</v>
+      </c>
+      <c r="G14" s="9">
+        <v>1</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>184</v>
+      </c>
       <c r="L14" s="8"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="9"/>
-      <c r="Q14" s="9"/>
-      <c r="R14" s="9"/>
-      <c r="S14" s="9"/>
-      <c r="T14" s="10"/>
-      <c r="U14" s="11"/>
-      <c r="V14" s="9"/>
-      <c r="W14" s="9"/>
-      <c r="X14" s="9"/>
-      <c r="Y14" s="9"/>
-      <c r="Z14" s="4"/>
-      <c r="AA14" s="4"/>
-      <c r="AB14" s="9"/>
-      <c r="AC14" s="9"/>
-      <c r="AD14" s="9"/>
-      <c r="AE14" s="9"/>
-      <c r="AF14" s="9"/>
-      <c r="AG14" s="9"/>
-      <c r="AH14" s="9"/>
-      <c r="AI14" s="9"/>
-      <c r="AJ14" s="9"/>
-      <c r="AK14" s="9"/>
+      <c r="M14" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="N14" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="O14" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="P14" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q14" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="R14" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="S14" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="T14" s="10">
+        <v>7.5231481481481477E-3</v>
+      </c>
+      <c r="U14" s="11">
+        <v>7.6388888888888886E-3</v>
+      </c>
+      <c r="V14" s="9">
+        <v>2012</v>
+      </c>
+      <c r="W14" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="X14" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y14" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z14" s="4">
+        <v>44409</v>
+      </c>
+      <c r="AA14" s="4">
+        <v>45138</v>
+      </c>
+      <c r="AB14" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC14" s="9">
+        <v>31028</v>
+      </c>
+      <c r="AD14" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE14" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF14" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="AG14" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="AH14" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI14" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="AJ14" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK14" s="9" t="s">
+        <v>88</v>
+      </c>
       <c r="AL14" s="8"/>
-      <c r="AM14" s="9"/>
-      <c r="AN14" s="9"/>
-      <c r="AO14" s="9"/>
-      <c r="AP14" s="9"/>
-      <c r="AQ14" s="9"/>
-      <c r="AR14" s="9"/>
-      <c r="AS14" s="9"/>
-      <c r="AT14" s="14"/>
-      <c r="AU14" s="9"/>
-      <c r="AV14" s="9"/>
+      <c r="AM14" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="AN14" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="AO14" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="AP14" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ14" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="AR14" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="AS14" s="9">
+        <v>610643928</v>
+      </c>
+      <c r="AT14" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="AU14" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="AV14" s="9" t="s">
+        <v>269</v>
+      </c>
       <c r="AW14" s="8"/>
-      <c r="AX14" s="9"/>
-      <c r="AY14" s="9"/>
-      <c r="AZ14" s="9"/>
+      <c r="AX14" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AY14" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AZ14" s="9" t="s">
+        <v>90</v>
+      </c>
       <c r="BA14" s="8"/>
-      <c r="BB14" s="9"/>
-      <c r="BC14" s="9"/>
-      <c r="BD14" s="9"/>
-      <c r="BE14" s="9"/>
-      <c r="BF14" s="9"/>
+      <c r="BB14" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="BC14" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="BD14" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="BE14" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="BF14" s="9" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="15" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
+      <c r="A15" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="B15" s="12">
+        <v>44623</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" s="9">
+        <v>1</v>
+      </c>
+      <c r="G15" s="9">
+        <v>1</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="J15" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="K15" s="9" t="s">
+        <v>193</v>
+      </c>
       <c r="L15" s="8"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="9"/>
-      <c r="P15" s="9"/>
-      <c r="Q15" s="9"/>
-      <c r="R15" s="9"/>
-      <c r="S15" s="9"/>
-      <c r="T15" s="10"/>
-      <c r="U15" s="11"/>
-      <c r="V15" s="9"/>
-      <c r="W15" s="9"/>
-      <c r="X15" s="9"/>
-      <c r="Y15" s="9"/>
-      <c r="Z15" s="4"/>
-      <c r="AA15" s="4"/>
-      <c r="AB15" s="9"/>
-      <c r="AC15" s="9"/>
-      <c r="AD15" s="9"/>
-      <c r="AE15" s="9"/>
-      <c r="AF15" s="9"/>
-      <c r="AG15" s="9"/>
-      <c r="AH15" s="9"/>
-      <c r="AI15" s="9"/>
-      <c r="AJ15" s="9"/>
-      <c r="AK15" s="9"/>
+      <c r="M15" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="N15" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="O15" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="P15" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="Q15" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="R15" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="S15" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="T15" s="10">
+        <v>7.5231481481481477E-3</v>
+      </c>
+      <c r="U15" s="11">
+        <v>7.6388888888888886E-3</v>
+      </c>
+      <c r="V15" s="9">
+        <v>2012</v>
+      </c>
+      <c r="W15" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="X15" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y15" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z15" s="4">
+        <v>44409</v>
+      </c>
+      <c r="AA15" s="4">
+        <v>45138</v>
+      </c>
+      <c r="AB15" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC15" s="9">
+        <v>31028</v>
+      </c>
+      <c r="AD15" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE15" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF15" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="AG15" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="AH15" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI15" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="AJ15" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK15" s="9" t="s">
+        <v>88</v>
+      </c>
       <c r="AL15" s="8"/>
-      <c r="AM15" s="9"/>
-      <c r="AN15" s="9"/>
-      <c r="AO15" s="9"/>
-      <c r="AP15" s="9"/>
-      <c r="AQ15" s="9"/>
-      <c r="AR15" s="9"/>
-      <c r="AS15" s="9"/>
-      <c r="AT15" s="9"/>
-      <c r="AU15" s="9"/>
-      <c r="AV15" s="9"/>
+      <c r="AM15" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="AN15" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="AO15" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="AP15" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ15" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="AR15" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="AS15" s="9">
+        <v>610643928</v>
+      </c>
+      <c r="AT15" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="AU15" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="AV15" s="9" t="s">
+        <v>273</v>
+      </c>
       <c r="AW15" s="8"/>
-      <c r="AX15" s="9"/>
-      <c r="AY15" s="9"/>
-      <c r="AZ15" s="9"/>
+      <c r="AX15" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AY15" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AZ15" s="9" t="s">
+        <v>90</v>
+      </c>
       <c r="BA15" s="8"/>
-      <c r="BB15" s="9"/>
-      <c r="BC15" s="9"/>
-      <c r="BD15" s="9"/>
-      <c r="BE15" s="9"/>
-      <c r="BF15" s="9"/>
+      <c r="BB15" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="BC15" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="BD15" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="BE15" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="BF15" s="9" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="16" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
+      <c r="A16" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="B16" s="12">
+        <v>44623</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="9">
+        <v>1</v>
+      </c>
+      <c r="G16" s="9">
+        <v>1</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="J16" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="K16" s="9" t="s">
+        <v>202</v>
+      </c>
       <c r="L16" s="8"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="9"/>
-      <c r="P16" s="9"/>
-      <c r="Q16" s="9"/>
-      <c r="R16" s="9"/>
-      <c r="S16" s="9"/>
-      <c r="T16" s="10"/>
-      <c r="U16" s="11"/>
-      <c r="V16" s="9"/>
-      <c r="W16" s="9"/>
-      <c r="X16" s="9"/>
-      <c r="Y16" s="9"/>
-      <c r="Z16" s="4"/>
-      <c r="AA16" s="4"/>
-      <c r="AB16" s="9"/>
-      <c r="AC16" s="9"/>
-      <c r="AD16" s="9"/>
-      <c r="AE16" s="9"/>
-      <c r="AF16" s="9"/>
-      <c r="AG16" s="9"/>
-      <c r="AH16" s="9"/>
-      <c r="AI16" s="9"/>
-      <c r="AJ16" s="9"/>
-      <c r="AK16" s="9"/>
+      <c r="M16" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="N16" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="O16" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="P16" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="Q16" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="R16" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="S16" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="T16" s="10">
+        <v>7.5231481481481477E-3</v>
+      </c>
+      <c r="U16" s="11">
+        <v>7.6388888888888886E-3</v>
+      </c>
+      <c r="V16" s="9">
+        <v>2012</v>
+      </c>
+      <c r="W16" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="X16" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y16" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z16" s="4">
+        <v>44409</v>
+      </c>
+      <c r="AA16" s="4">
+        <v>45138</v>
+      </c>
+      <c r="AB16" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC16" s="9">
+        <v>31028</v>
+      </c>
+      <c r="AD16" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE16" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF16" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="AG16" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="AH16" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI16" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="AJ16" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK16" s="9" t="s">
+        <v>88</v>
+      </c>
       <c r="AL16" s="8"/>
-      <c r="AM16" s="9"/>
-      <c r="AN16" s="9"/>
-      <c r="AO16" s="9"/>
-      <c r="AP16" s="9"/>
-      <c r="AQ16" s="9"/>
-      <c r="AR16" s="9"/>
-      <c r="AS16" s="9"/>
-      <c r="AT16" s="9"/>
-      <c r="AU16" s="9"/>
-      <c r="AV16" s="9"/>
+      <c r="AM16" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="AN16" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="AO16" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="AP16" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ16" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="AR16" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="AS16" s="9">
+        <v>610643928</v>
+      </c>
+      <c r="AT16" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="AU16" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="AV16" s="9" t="s">
+        <v>277</v>
+      </c>
       <c r="AW16" s="8"/>
-      <c r="AX16" s="9"/>
-      <c r="AY16" s="9"/>
-      <c r="AZ16" s="9"/>
+      <c r="AX16" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AY16" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AZ16" s="9" t="s">
+        <v>90</v>
+      </c>
       <c r="BA16" s="8"/>
-      <c r="BB16" s="9"/>
-      <c r="BC16" s="9"/>
-      <c r="BD16" s="9"/>
-      <c r="BE16" s="9"/>
-      <c r="BF16" s="9"/>
+      <c r="BB16" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="BC16" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="BD16" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="BE16" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="BF16" s="9" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="17" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
+      <c r="A17" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="B17" s="12">
+        <v>44623</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" s="9">
+        <v>1</v>
+      </c>
+      <c r="G17" s="9">
+        <v>1</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="J17" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="K17" s="9" t="s">
+        <v>211</v>
+      </c>
       <c r="L17" s="8"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="9"/>
-      <c r="P17" s="9"/>
-      <c r="Q17" s="9"/>
-      <c r="R17" s="9"/>
-      <c r="S17" s="9"/>
-      <c r="T17" s="10"/>
-      <c r="U17" s="11"/>
-      <c r="V17" s="9"/>
-      <c r="W17" s="9"/>
-      <c r="X17" s="9"/>
-      <c r="Y17" s="9"/>
-      <c r="Z17" s="4"/>
-      <c r="AA17" s="4"/>
-      <c r="AB17" s="9"/>
-      <c r="AC17" s="9"/>
-      <c r="AD17" s="9"/>
-      <c r="AE17" s="9"/>
-      <c r="AF17" s="9"/>
-      <c r="AG17" s="9"/>
-      <c r="AH17" s="9"/>
-      <c r="AI17" s="9"/>
-      <c r="AJ17" s="9"/>
-      <c r="AK17" s="9"/>
+      <c r="M17" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="N17" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="O17" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="P17" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="Q17" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="R17" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="S17" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="T17" s="10">
+        <v>7.5231481481481477E-3</v>
+      </c>
+      <c r="U17" s="11">
+        <v>7.6388888888888886E-3</v>
+      </c>
+      <c r="V17" s="9">
+        <v>2012</v>
+      </c>
+      <c r="W17" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="X17" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y17" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z17" s="4">
+        <v>44409</v>
+      </c>
+      <c r="AA17" s="4">
+        <v>45138</v>
+      </c>
+      <c r="AB17" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC17" s="9">
+        <v>31028</v>
+      </c>
+      <c r="AD17" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE17" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF17" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="AG17" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="AH17" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI17" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="AJ17" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK17" s="9" t="s">
+        <v>88</v>
+      </c>
       <c r="AL17" s="8"/>
-      <c r="AM17" s="9"/>
-      <c r="AN17" s="9"/>
-      <c r="AO17" s="9"/>
-      <c r="AP17" s="9"/>
-      <c r="AQ17" s="9"/>
-      <c r="AR17" s="9"/>
-      <c r="AS17" s="9"/>
-      <c r="AT17" s="9"/>
-      <c r="AU17" s="9"/>
-      <c r="AV17" s="9"/>
+      <c r="AM17" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="AN17" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="AO17" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="AP17" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ17" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="AR17" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="AS17" s="9">
+        <v>610643928</v>
+      </c>
+      <c r="AT17" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="AU17" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="AV17" s="9" t="s">
+        <v>281</v>
+      </c>
       <c r="AW17" s="8"/>
-      <c r="AX17" s="9"/>
-      <c r="AY17" s="9"/>
-      <c r="AZ17" s="9"/>
+      <c r="AX17" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AY17" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AZ17" s="9" t="s">
+        <v>90</v>
+      </c>
       <c r="BA17" s="8"/>
-      <c r="BB17" s="9"/>
-      <c r="BC17" s="9"/>
-      <c r="BD17" s="9"/>
-      <c r="BE17" s="9"/>
-      <c r="BF17" s="9"/>
+      <c r="BB17" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="BC17" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="BD17" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="BE17" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="BF17" s="9" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="18" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>

</xml_diff>

<commit_message>
Serie Las Aventuras de Wibbly SD Y HD
</commit_message>
<xml_diff>
--- a/XML_SD_HD.xlsx
+++ b/XML_SD_HD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Readfile\createReadFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2619C854-B835-4A81-8517-14D2E1EDBE17}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FB5999B-4F94-445C-9BF9-3C76BBEA1018}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -276,605 +276,604 @@
     <t>EP 26</t>
   </si>
   <si>
-    <t>EEMMMT111_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEMM6000000000000111</t>
-  </si>
-  <si>
-    <t>Serie Las Aventuras de Meteor</t>
-  </si>
-  <si>
-    <t>Las Aventuras de MeteorT01EP11</t>
-  </si>
-  <si>
-    <t>Las Aventuras de Meteor T01 EP11</t>
-  </si>
-  <si>
-    <t>Edye presenta: Para no participar en una carrera que considera difícil, Amby finge estar enfermo.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Para evitar participar en la última carrera de contrarreloj de Big Wheelie, Amby finge que está enfermo porque cree que la competencia es demasiado difícil para un pequeño camión monstruo como él.</t>
-  </si>
-  <si>
-    <t>Infantil/Las Aventuras de Meteor</t>
-  </si>
-  <si>
-    <t>Las Aventuras de Meteor</t>
-  </si>
-  <si>
-    <t>USA</t>
-  </si>
-  <si>
-    <t>Ansell Cameron, Eisner Mitchell, Isen Tajja, Petronijevic Dan, Saunders Cliff</t>
-  </si>
-  <si>
-    <t>Meteor the Monster</t>
-  </si>
-  <si>
-    <t>Hierons, Trevor</t>
-  </si>
-  <si>
-    <t>EEMMMT111.mpg</t>
-  </si>
-  <si>
-    <t>EEMMMT1_box.jpg</t>
-  </si>
-  <si>
-    <t>EEMMMT111_land.jpg</t>
-  </si>
-  <si>
-    <t>EEMMMT112_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEMM6000000000000112</t>
-  </si>
-  <si>
-    <t>Las Aventuras de MeteorT01EP12</t>
-  </si>
-  <si>
-    <t>Las Aventuras de Meteor T01 EP12</t>
-  </si>
-  <si>
-    <t>Edye presenta: Meteoro está molesto con Basurita porque lo abandonó cuando estaba en problemas.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Basurita deja a Meteoro atrapado en un charco de lodo muy profundo ¡Meteoro no puede creer que su amigo se haya ido! y, sólo es hasta que Basurita finalmente admite lo que hizo, se da cuenta de que en realidad él no tenía la culpa del accidente.</t>
-  </si>
-  <si>
-    <t>EEMMMT112.mpg</t>
-  </si>
-  <si>
-    <t>EEMMMT112_land.jpg</t>
-  </si>
-  <si>
-    <t>EEMMMT113_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEMM6000000000000113</t>
-  </si>
-  <si>
-    <t>Las Aventuras de MeteorT01EP13</t>
-  </si>
-  <si>
-    <t>Las Aventuras de Meteor T01 EP13</t>
-  </si>
-  <si>
-    <t>Edye presenta: Durante una exhibición, Meteoro está a punto de causar un problema por no hacer su trabajo.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Crushmeister, uno de los camiones monstruo más famosos de Crushington Park se va a presentar y Meteoro se ofrece para ayudar durante el evento. Sin embargo, se distrae jugando con sus amigos y Big Wheelie tiene que intervenir para evitar un problema.</t>
-  </si>
-  <si>
-    <t>EEMMMT113.mpg</t>
-  </si>
-  <si>
-    <t>EEMMMT113_land.jpg</t>
-  </si>
-  <si>
-    <t>EEMMMT114_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEMM6000000000000114</t>
-  </si>
-  <si>
-    <t>Las Aventuras de MeteorT01EP14</t>
-  </si>
-  <si>
-    <t>Las Aventuras de Meteor T01 EP14</t>
-  </si>
-  <si>
-    <t>Edye presenta: Cuando Big Wheelie le encarga una tarea a Meteoro, este debe aprender cómo ser un buen líder.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Meteoro debe aprender a no ser un líder mandón cuando Big Wheelie lo elige para dirigir a sus amigos en la creación de una nueva “Línea de Meta” para la pista de carreras de la escuela.</t>
-  </si>
-  <si>
-    <t>EEMMMT114.mpg</t>
-  </si>
-  <si>
-    <t>EEMMMT114_land.jpg</t>
-  </si>
-  <si>
-    <t>EEMMMT115_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEMM6000000000000115</t>
-  </si>
-  <si>
-    <t>Las Aventuras de MeteorT01EP15</t>
-  </si>
-  <si>
-    <t>Las Aventuras de Meteor T01 EP15</t>
-  </si>
-  <si>
-    <t>Edye presenta: Meteoro aprende que hay que practicar hasta que las cosas salgan bien.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Meteoro comprende que si algo no le sale bien la primera vez, practicar y practicar, es lo que lo convertirá en un experto.</t>
-  </si>
-  <si>
-    <t>EEMMMT115.mpg</t>
-  </si>
-  <si>
-    <t>EEMMMT115_land.jpg</t>
-  </si>
-  <si>
-    <t>EEMMMT116_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEMM6000000000000116</t>
-  </si>
-  <si>
-    <t>Las Aventuras de MeteorT01EP16</t>
-  </si>
-  <si>
-    <t>Las Aventuras de Meteor T01 EP16</t>
-  </si>
-  <si>
-    <t>Edye presenta: Meteoro se preocupa pensando que las historias del abuelo aburrirán a sus amigos.</t>
-  </si>
-  <si>
-    <t>Edye presenta: El héroe de Meteoro viene de visita: ¡su abuelo, el vehículo lunar original! Pero, cuando queda claro que ya han pasado los días de gloria del abuelo, Meteoro se preocupa innecesariamente pensando que las historias del abuelo aburrirán a sus amigos.</t>
-  </si>
-  <si>
-    <t>EEMMMT116.mpg</t>
-  </si>
-  <si>
-    <t>EEMMMT116_land.jpg</t>
-  </si>
-  <si>
-    <t>EEMMMT117_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEMM6000000000000117</t>
-  </si>
-  <si>
-    <t>Las Aventuras de MeteorT01EP17</t>
-  </si>
-  <si>
-    <t>Las Aventuras de Meteor T01 EP17</t>
-  </si>
-  <si>
-    <t>Edye presenta: Meteoro tiene el temor de que una de sus pesadillas se convierta en realidad.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Meteoro tiene problemas para olvidar la pesadilla que tuvo: Basurita lo empujaba a una zanja al costado del camino. Por lo que, al día siguiente, Meteoro evita a su amigo por temor a que su mal sueño se haga realidad.</t>
-  </si>
-  <si>
-    <t>EEMMMT117.mpg</t>
-  </si>
-  <si>
-    <t>EEMMMT117_land.jpg</t>
-  </si>
-  <si>
-    <t>EEMMMT118_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEMM6000000000000118</t>
-  </si>
-  <si>
-    <t>Las Aventuras de MeteorT01EP18</t>
-  </si>
-  <si>
-    <t>Las Aventuras de Meteor T01 EP18</t>
-  </si>
-  <si>
-    <t>Edye presenta: Meteoro aprende la importancia de no depender únicamente de la tecnología.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Meteoro entiende lo importante que es aprender los conceptos básicos en lugar de depender de la tecnología, cuando daña por accidente un pantalla de video que iba a usar para ganar "la carrera hacia atrás", un recorrido totalmente en reversa.</t>
-  </si>
-  <si>
-    <t>EEMMMT118.mpg</t>
-  </si>
-  <si>
-    <t>EEMMMT118_land.jpg</t>
-  </si>
-  <si>
-    <t>EEMMMT119_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEMM6000000000000119</t>
-  </si>
-  <si>
-    <t>Las Aventuras de MeteorT01EP19</t>
-  </si>
-  <si>
-    <t>Las Aventuras de Meteor T01 EP19</t>
-  </si>
-  <si>
-    <t>Edye presenta: Pequeñín quiere usar un enorme gancho pero se da cuenta de que no corresponde a su tamaño.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Pequeñín se enamora de un gancho remolcador que encontró en su patio. Pero cuando intenta usar el enorme gancho para sacar a uno de sus amigos de la basura, se da cuenta de que aun es pequeño para usarlo y no hay nada que pueda hacer al respecto.</t>
-  </si>
-  <si>
-    <t>EEMMMT119.mpg</t>
-  </si>
-  <si>
-    <t>EEMMMT119_land.jpg</t>
-  </si>
-  <si>
-    <t>EEMMMT120_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEMM6000000000000120</t>
-  </si>
-  <si>
-    <t>Las Aventuras de MeteorT01EP20</t>
-  </si>
-  <si>
-    <t>Las Aventuras de Meteor T01 EP20</t>
-  </si>
-  <si>
-    <t>Edye presenta: Meteoro se molesta con sus amigos cuando comienzan a actuar de forma misteriosa.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Meteoro se molesta porque sus amigos lo evitan cuando están jugando al escondite, hasta que descubre que actuaban de forma misteriosa porque le estaban organizando una fiesta de cumpleaños sorpresa.</t>
-  </si>
-  <si>
-    <t>EEMMMT120.mpg</t>
-  </si>
-  <si>
-    <t>EEMMMT120_land.jpg</t>
-  </si>
-  <si>
-    <t>EEMMMT121_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEMM6000000000000121</t>
-  </si>
-  <si>
-    <t>Las Aventuras de MeteorT01EP21</t>
-  </si>
-  <si>
-    <t>Las Aventuras de Meteor T01 EP21</t>
-  </si>
-  <si>
-    <t>Edye presenta: Big Wheelie les da a los camiones una lección sobre la importancia de seguir las instrucciones.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Big Wheelie les da a los camiones una lección sobre la importancia de seguir las instrucciones cuando organiza una carrera para que los chicos recorran un laberinto con distracciones en cada vuelta.</t>
-  </si>
-  <si>
-    <t>EEMMMT121.mpg</t>
-  </si>
-  <si>
-    <t>EEMMMT121_land.jpg</t>
-  </si>
-  <si>
-    <t>EEMMMT122_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEMM6000000000000122</t>
-  </si>
-  <si>
-    <t>Las Aventuras de MeteorT01EP22</t>
-  </si>
-  <si>
-    <t>Las Aventuras de Meteor T01 EP22</t>
-  </si>
-  <si>
-    <t>Edye presenta: Pony les demuesta a los demás que deben darles una oportunidad a alguien que es diferente a ti.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Sue, un camión de apoyo apestoso y de mal carácter, no les cae bien al resto de los camiones, hasta que Pony se hace amiga de ella y todos aprenden el valor de acercarse a alguien que es diferente a ti.</t>
-  </si>
-  <si>
-    <t>EEMMMT122.mpg</t>
-  </si>
-  <si>
-    <t>EEMMMT122_land.jpg</t>
-  </si>
-  <si>
-    <t>EEMMMT123_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEMM6000000000000123</t>
-  </si>
-  <si>
-    <t>Las Aventuras de MeteorT01EP23</t>
-  </si>
-  <si>
-    <t>Las Aventuras de Meteor T01 EP23</t>
-  </si>
-  <si>
-    <t>Edye presenta: Meteoro aprende que se puede ser un gran vehículo espacial, aunque no gane todas las carreras.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Meteoro aprende que se puede ser un gran vehículo espacial, a pesar de no ganar todas las carreras, cuando Cosmo Starfinder, uno de sus héroes espaciales, hace correr a los pequeños camiones durante un recorrido de entrenamiento en la escuela.</t>
-  </si>
-  <si>
-    <t>EEMMMT123.mpg</t>
-  </si>
-  <si>
-    <t>EEMMMT123_land.jpg</t>
-  </si>
-  <si>
-    <t>EEMMMT124_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEMM6000000000000124</t>
-  </si>
-  <si>
-    <t>Las Aventuras de MeteorT01EP24</t>
-  </si>
-  <si>
-    <t>Las Aventuras de Meteor T01 EP24</t>
-  </si>
-  <si>
-    <t>Edye presenta: Pony se va a dar una vuelta con su primo sin avisar a sus padres y aprenderá una lección.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Duke, un viejo camión de rodeo, primo de Pony llega a la escuela de Crushington Park. Al terminar las clases, los dos se van a dar una vuelta. Pony aprende la importancia de avisar siempre a sus padres en dónde se encuentra.</t>
-  </si>
-  <si>
-    <t>EEMMMT124.mpg</t>
-  </si>
-  <si>
-    <t>EEMMMT124_land.jpg</t>
-  </si>
-  <si>
-    <t>EEMMMT125_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEMM6000000000000125</t>
-  </si>
-  <si>
-    <t>Las Aventuras de MeteorT01EP25</t>
-  </si>
-  <si>
-    <t>Las Aventuras de Meteor T01 EP25</t>
-  </si>
-  <si>
-    <t>Edye presenta: Todos los chicos quieren salir en la televisión, pero Pony, por su actitud es la elegida.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Edye presenta: Dynamite Dan, la camioneta de la televisión ha llegado al pueblo para hacer un reportaje. Todos los chicos quieren impresionar a Dan demostrando sus habilidades pero es Pony, con su actitud tranquila, quien es elegida para aparecer en televisión.
-</t>
-  </si>
-  <si>
-    <t>EEMMMT125.mpg</t>
-  </si>
-  <si>
-    <t>EEMMMT125_land.jpg</t>
-  </si>
-  <si>
-    <t>EEMMMT126_SD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEMM6000000000000126</t>
-  </si>
-  <si>
-    <t>Las Aventuras de MeteorT01EP26</t>
-  </si>
-  <si>
-    <t>Las Aventuras de Meteor T01 EP26</t>
-  </si>
-  <si>
-    <t>Edye presenta: Los pequeños camiones deberán aprender a adaptarse a los cambios inesperados en su rutina.</t>
-  </si>
-  <si>
-    <t>Edye presenta: Big Wheelie va a participar en una carrera y en su ausencia, un vehículo militar, el Sr Halftrack, se hará cargo de la clase. Los pequeños camiones deberán aprender a adaptarse a los cambios inesperados en su rutina diaria.</t>
-  </si>
-  <si>
-    <t>EEMMMT126.mpg</t>
-  </si>
-  <si>
-    <t>EEMMMT126_land.jpg</t>
-  </si>
-  <si>
-    <t>EEMMMT111_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEMM7000000000000111</t>
-  </si>
-  <si>
-    <t>Las Aventuras de Meteor T01 EP11 HD</t>
-  </si>
-  <si>
-    <t>EEMMMT111.ts</t>
-  </si>
-  <si>
-    <t>EEMMMT112_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEMM7000000000000112</t>
-  </si>
-  <si>
-    <t>Las Aventuras de Meteor T01 EP12 HD</t>
-  </si>
-  <si>
-    <t>EEMMMT112.ts</t>
-  </si>
-  <si>
-    <t>EEMMMT113_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEMM7000000000000113</t>
-  </si>
-  <si>
-    <t>Las Aventuras de Meteor T01 EP13 HD</t>
-  </si>
-  <si>
-    <t>EEMMMT113.ts</t>
-  </si>
-  <si>
-    <t>EEMMMT114_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEMM7000000000000114</t>
-  </si>
-  <si>
-    <t>Las Aventuras de Meteor T01 EP14 HD</t>
-  </si>
-  <si>
-    <t>EEMMMT114.ts</t>
-  </si>
-  <si>
-    <t>EEMMMT115_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEMM7000000000000115</t>
-  </si>
-  <si>
-    <t>Las Aventuras de Meteor T01 EP15 HD</t>
-  </si>
-  <si>
-    <t>EEMMMT115.ts</t>
-  </si>
-  <si>
-    <t>EEMMMT116_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEMM7000000000000116</t>
-  </si>
-  <si>
-    <t>Las Aventuras de Meteor T01 EP16 HD</t>
-  </si>
-  <si>
-    <t>EEMMMT116.ts</t>
-  </si>
-  <si>
-    <t>EEMMMT117_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEMM7000000000000117</t>
-  </si>
-  <si>
-    <t>Las Aventuras de Meteor T01 EP17 HD</t>
-  </si>
-  <si>
-    <t>EEMMMT117.ts</t>
-  </si>
-  <si>
-    <t>EEMMMT118_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEMM7000000000000118</t>
-  </si>
-  <si>
-    <t>Las Aventuras de Meteor T01 EP18 HD</t>
-  </si>
-  <si>
-    <t>EEMMMT118.ts</t>
-  </si>
-  <si>
-    <t>EEMMMT119_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEMM7000000000000119</t>
-  </si>
-  <si>
-    <t>Las Aventuras de Meteor T01 EP19 HD</t>
-  </si>
-  <si>
-    <t>EEMMMT119.ts</t>
-  </si>
-  <si>
-    <t>EEMMMT120_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEMM7000000000000120</t>
-  </si>
-  <si>
-    <t>Las Aventuras de Meteor T01 EP20 HD</t>
-  </si>
-  <si>
-    <t>EEMMMT120.ts</t>
-  </si>
-  <si>
-    <t>EEMMMT121_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEMM7000000000000121</t>
-  </si>
-  <si>
-    <t>Las Aventuras de Meteor T01 EP21 HD</t>
-  </si>
-  <si>
-    <t>EEMMMT121.ts</t>
-  </si>
-  <si>
-    <t>EEMMMT122_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEMM7000000000000122</t>
-  </si>
-  <si>
-    <t>Las Aventuras de Meteor T01 EP22 HD</t>
-  </si>
-  <si>
-    <t>EEMMMT122.ts</t>
-  </si>
-  <si>
-    <t>EEMMMT123_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEMM7000000000000123</t>
-  </si>
-  <si>
-    <t>Las Aventuras de Meteor T01 EP23 HD</t>
-  </si>
-  <si>
-    <t>EEMMMT123.ts</t>
-  </si>
-  <si>
-    <t>EEMMMT124_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEMM7000000000000124</t>
-  </si>
-  <si>
-    <t>Las Aventuras de Meteor T01 EP24 HD</t>
-  </si>
-  <si>
-    <t>EEMMMT124.ts</t>
-  </si>
-  <si>
-    <t>EEMMMT125_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEMM7000000000000125</t>
-  </si>
-  <si>
-    <t>Las Aventuras de Meteor T01 EP25 HD</t>
-  </si>
-  <si>
-    <t>EEMMMT125.ts</t>
-  </si>
-  <si>
-    <t>EEMMMT126_HD_ADI.XML</t>
-  </si>
-  <si>
-    <t>EEMM7000000000000126</t>
-  </si>
-  <si>
-    <t>Las Aventuras de Meteor T01 EP26 HD</t>
-  </si>
-  <si>
-    <t>EEMMMT126.ts</t>
+    <t>EEWPIG111_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEWP6000000000000111</t>
+  </si>
+  <si>
+    <t>Serie Las Aventuras de Wibbly</t>
+  </si>
+  <si>
+    <t>Las Aventuras de WibblyT01EP11</t>
+  </si>
+  <si>
+    <t>Las Aventuras de Wibbly T01 EP11</t>
+  </si>
+  <si>
+    <t>Edye presenta: ¿Qué tipo de música te hace querer menearte y bailar? ¡A todos nos gustan cosas diferentes!</t>
+  </si>
+  <si>
+    <t>Edye presenta: ¿Qué tipo de música te hace querer menearte y bailar? ¡A todos nos gustan las cosas diferentes! Wibbly parece que no puede encontrar la música correcta pero ¡Al final, Wibbly y sus amigos ponen toda tipo de música y bailan!</t>
+  </si>
+  <si>
+    <t>Infantil/Las Aventuras de Wibbly</t>
+  </si>
+  <si>
+    <t>Las Aventuras de Wibbly</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>Liam Tully, Deo Simcox, Mark Ramsay, Zoe Fraser, Jacob Ewaniuk</t>
+  </si>
+  <si>
+    <t>WP Productions</t>
+  </si>
+  <si>
+    <t>Tully Liam, Simcox Deo, Ramsay Mark, Fraser Zoe, Ewaniuk Jacob</t>
+  </si>
+  <si>
+    <t>Hall, Jez</t>
+  </si>
+  <si>
+    <t>EEWPIG111.mpg</t>
+  </si>
+  <si>
+    <t>EEWPIG1_box.jpg</t>
+  </si>
+  <si>
+    <t>EEWPIG111_land.jpg</t>
+  </si>
+  <si>
+    <t>EEWPIG112_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEWP6000000000000112</t>
+  </si>
+  <si>
+    <t>Las Aventuras de WibblyT01EP12</t>
+  </si>
+  <si>
+    <t>Las Aventuras de Wibbly T01 EP12</t>
+  </si>
+  <si>
+    <t>Edye presenta: ¡Wibbly y Tiny Pig hacen un bote! Sólo tenemos que esperar viento para comenzar la aventura.</t>
+  </si>
+  <si>
+    <t>Edye presenta: ¡Wibbly y Tiny Pig hacen un bote! Wibbly dibuja un mapa a medida que avanzamos. En el camino el viento se levanta y nos lleva a una isla desierta donde nos encontramos con Scruffy Pig ¡Ahora sólo tenemos que esperar un buen viento para volver a casa!</t>
+  </si>
+  <si>
+    <t>EEWPIG112.mpg</t>
+  </si>
+  <si>
+    <t>EEWPIG112_land.jpg</t>
+  </si>
+  <si>
+    <t>EEWPIG113_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEWP6000000000000113</t>
+  </si>
+  <si>
+    <t>Las Aventuras de WibblyT01EP13</t>
+  </si>
+  <si>
+    <t>Las Aventuras de Wibbly T01 EP13</t>
+  </si>
+  <si>
+    <t>Edye presenta: Wibbly está jugando en una tienda de campaña y Pigley desaparece antes de comenzar el viaje.</t>
+  </si>
+  <si>
+    <t>Edye presenta: Todos juegan a esconderse. La regla dice que a quién encuentren al último, será el siguiente en buscar, pero como todos se esconden juntos, cuando Wibbly Pig los encuentra, nadie fue “el último” por lo que Wibbly ¡tiene que seguir buscando!</t>
+  </si>
+  <si>
+    <t>EEWPIG113.mpg</t>
+  </si>
+  <si>
+    <t>EEWPIG113_land.jpg</t>
+  </si>
+  <si>
+    <t>EEWPIG114_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEWP6000000000000114</t>
+  </si>
+  <si>
+    <t>Las Aventuras de WibblyT01EP14</t>
+  </si>
+  <si>
+    <t>Las Aventuras de Wibbly T01 EP14</t>
+  </si>
+  <si>
+    <t>Edye presenta: A Wibbly le gusta conducir su coche pero al viajar con Pigley hay obstáculos en el camino.</t>
+  </si>
+  <si>
+    <t>Edye presenta: A Wibbly le gusta conducir en su automóvil pero a pesar de sus mejores esfuerzos para llevar a Pigley a un lindo viaje, descubre que los Pig Twins parecen amar la velocidad, Scruffy Pig levanta una nube de polvo y Tiny Pig causa un atasco de tráfico.</t>
+  </si>
+  <si>
+    <t>EEWPIG114.mpg</t>
+  </si>
+  <si>
+    <t>EEWPIG114_land.jpg</t>
+  </si>
+  <si>
+    <t>EEWPIG115_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEWP6000000000000115</t>
+  </si>
+  <si>
+    <t>Las Aventuras de WibblyT01EP15</t>
+  </si>
+  <si>
+    <t>Las Aventuras de Wibbly T01 EP15</t>
+  </si>
+  <si>
+    <t>Edye presenta: Wibbly y sus amigos inician un viaje espacial en el que encuentran un universo y nuevos amigos</t>
+  </si>
+  <si>
+    <t>Edye presenta: Cuando Wibbly y sus amigos inician su viaje espacial, su cuarto es un desastre. En su viaje se encuentran en un universo en el sus nuevos amigos ordenan la galaxia y cuando regresan a la tierra ¡encuentran que la habitación también ha sido ordenada!</t>
+  </si>
+  <si>
+    <t>EEWPIG115.mpg</t>
+  </si>
+  <si>
+    <t>EEWPIG115_land.jpg</t>
+  </si>
+  <si>
+    <t>EEWPIG116_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEWP6000000000000116</t>
+  </si>
+  <si>
+    <t>Las Aventuras de WibblyT01EP16</t>
+  </si>
+  <si>
+    <t>Las Aventuras de Wibbly T01 EP16</t>
+  </si>
+  <si>
+    <t>Edye presenta: Wibbly tiene un nuevo soplador de burbujas y todos pueden soplar burbujas perfectas excepto él.</t>
+  </si>
+  <si>
+    <t>Edye presenta: Wibbly es el orgulloso propietario de un nuevo soplador de burbujas, ¡pero todos los demás pueden soplar burbujas perfectas excepto él! Cuando finalmente sopla algunas, forman una burbuja Wibbly, lo que lo lleva a una divertida aventura burbujeante.</t>
+  </si>
+  <si>
+    <t>EEWPIG116.mpg</t>
+  </si>
+  <si>
+    <t>EEWPIG116_land.jpg</t>
+  </si>
+  <si>
+    <t>EEWPIG117_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEWP6000000000000117</t>
+  </si>
+  <si>
+    <t>Las Aventuras de WibblyT01EP17</t>
+  </si>
+  <si>
+    <t>Las Aventuras de Wibbly T01 EP17</t>
+  </si>
+  <si>
+    <t>Edye presenta: Wibbly está jugando en una tienda de campaña. Pero antes de que pueda comenzar el viaje, Pigley desaparece. Nuestra búsqueda nos lleva al bosque, a la Antártida y a las montañas. Para cuando aparece Pigle ¡se ha comido todas las galletas!</t>
+  </si>
+  <si>
+    <t>EEWPIG117.mpg</t>
+  </si>
+  <si>
+    <t>EEWPIG117_land.jpg</t>
+  </si>
+  <si>
+    <t>EEWPIG118_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEWP6000000000000118</t>
+  </si>
+  <si>
+    <t>Las Aventuras de WibblyT01EP18</t>
+  </si>
+  <si>
+    <t>Las Aventuras de Wibbly T01 EP18</t>
+  </si>
+  <si>
+    <t>Edye presenta: Durante su nueva visita, la tía Larlie ha traido un gran regalo a Wibbly ¿Qué podrá ser?</t>
+  </si>
+  <si>
+    <t>Edye presenta: La tía Larlie, es muy divertida y le ha dado muchos regalos a Wibbly, aunque no todos le han gustado demasiado. Durante su nueva visita él está un poco nervioso porque ella lleva un gran regalo, pero cuando abre el presente, ¿qué encontrará?</t>
+  </si>
+  <si>
+    <t>EEWPIG118.mpg</t>
+  </si>
+  <si>
+    <t>EEWPIG118_land.jpg</t>
+  </si>
+  <si>
+    <t>EEWPIG119_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEWP6000000000000119</t>
+  </si>
+  <si>
+    <t>Las Aventuras de WibblyT01EP19</t>
+  </si>
+  <si>
+    <t>Las Aventuras de Wibbly T01 EP19</t>
+  </si>
+  <si>
+    <t>Edye presenta: Wibbly muestra con orgullo a Rocket, su nuevo caballo mecedor y está impaciente por montarlo.</t>
+  </si>
+  <si>
+    <t>Edye presenta: Wibbly muestra con orgullo a Rocket, su nuevo caballo mecedor. Wibbly no puede esperar para montarlo pero pronto se da cuenta de que no es tan fácil ser un vaquero. Junto con Tiny, aprenden a cabalgar e incluso logran reunir un poco de ganado.</t>
+  </si>
+  <si>
+    <t>EEWPIG119.mpg</t>
+  </si>
+  <si>
+    <t>EEWPIG119_land.jpg</t>
+  </si>
+  <si>
+    <t>EEWPIG120_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEWP6000000000000120</t>
+  </si>
+  <si>
+    <t>Las Aventuras de WibblyT01EP20</t>
+  </si>
+  <si>
+    <t>Las Aventuras de Wibbly T01 EP20</t>
+  </si>
+  <si>
+    <t>Edye presenta: Wibbly recuerda las cosas divertidas que ha hecho con su abuelo mientras espera su llegada.</t>
+  </si>
+  <si>
+    <t>Edye presenta: Wibbly está esperando a su abuelo. Mientras llega, Wibbly recuerda algunas de las cosas divertidas que han hecho juntos, porque él es el mejor abuelo del mundo, pero ¿por qué tarda tanto? Cuando aparece, ¡trae un nuevo juego divertido para él!</t>
+  </si>
+  <si>
+    <t>EEWPIG120.mpg</t>
+  </si>
+  <si>
+    <t>EEWPIG120_land.jpg</t>
+  </si>
+  <si>
+    <t>EEWPIG121_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEWP6000000000000121</t>
+  </si>
+  <si>
+    <t>Las Aventuras de WibblyT01EP21</t>
+  </si>
+  <si>
+    <t>Las Aventuras de Wibbly T01 EP21</t>
+  </si>
+  <si>
+    <t>Edye presenta: Wibbly nos presenta a su orquesta formada por todo tipo de animales pero, ¿Dónde los encontró?</t>
+  </si>
+  <si>
+    <t>Edye presenta: Wibbly nos presenta a su nueva orquesta formada por un pollo, un oso, algunos pájaros, dos elefantes y un ganso ¡La orquesta de Wibbly está completa! ¿Pero en dónde encontró Wibbly a todos estos animales?</t>
+  </si>
+  <si>
+    <t>EEWPIG121.mpg</t>
+  </si>
+  <si>
+    <t>EEWPIG121_land.jpg</t>
+  </si>
+  <si>
+    <t>EEWPIG122_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEWP6000000000000122</t>
+  </si>
+  <si>
+    <t>Las Aventuras de WibblyT01EP22</t>
+  </si>
+  <si>
+    <t>Las Aventuras de Wibbly T01 EP22</t>
+  </si>
+  <si>
+    <t>Edye presenta: ¡Wibbly se hizo un disfraz de robot! Y ninguno de los chicos logra descubrir quién es él.</t>
+  </si>
+  <si>
+    <t>Edye presenta: ¡Wibbly se hizo un disfraz de robot! Cuando Scruffy Pig viene a buscarlo, decidimos jugarle una mala pasada y ver si puede saber quién es realmente el robot. ¡No lo hace y tampoco Big Pig! Al final, todos hacen su propio robot y todos bailamos juntos</t>
+  </si>
+  <si>
+    <t>EEWPIG122.mpg</t>
+  </si>
+  <si>
+    <t>EEWPIG122_land.jpg</t>
+  </si>
+  <si>
+    <t>EEWPIG123_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEWP6000000000000123</t>
+  </si>
+  <si>
+    <t>Las Aventuras de WibblyT01EP23</t>
+  </si>
+  <si>
+    <t>Las Aventuras de Wibbly T01 EP23</t>
+  </si>
+  <si>
+    <t>Edye presenta: ¡Wibbly Pig, Big Pig y Tiny Pig están en la playa y van a hacer el mejor castillo de arena!</t>
+  </si>
+  <si>
+    <t>Edye presenta: ¡Wibbly Pig, Big Pig y Tiny Pig están en la playa y van a hacer el mejor castillo de arena! Pero no es tan sencillo como parece. Al final logran darle forma a la fortaleza pero ¿podrán proteger su castillo de las olas al subir la marea?</t>
+  </si>
+  <si>
+    <t>EEWPIG123.mpg</t>
+  </si>
+  <si>
+    <t>EEWPIG123_land.jpg</t>
+  </si>
+  <si>
+    <t>EEWPIG124_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEWP6000000000000124</t>
+  </si>
+  <si>
+    <t>Las Aventuras de WibblyT01EP24</t>
+  </si>
+  <si>
+    <t>Las Aventuras de Wibbly T01 EP24</t>
+  </si>
+  <si>
+    <t>Edye presenta: Wibbly y sus amigos hacen un cerdito de nieve y otras figuras de animales para jugar juntos.</t>
+  </si>
+  <si>
+    <t>Edye presenta: Afuera hace mucho frío y Wibbly Pig y sus amigos están haciendo bolas de nieve. Juntos hacen un cerdo de nieve, pero se les escapa y quiere jugar. Pero cuando es hora de entrar, los chicos hacen otras figuras para que el cerdo de nieve no esté solo.</t>
+  </si>
+  <si>
+    <t>EEWPIG124.mpg</t>
+  </si>
+  <si>
+    <t>EEWPIG124_land.jpg</t>
+  </si>
+  <si>
+    <t>EEWPIG125_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEWP6000000000000125</t>
+  </si>
+  <si>
+    <t>Las Aventuras de WibblyT01EP25</t>
+  </si>
+  <si>
+    <t>Las Aventuras de Wibbly T01 EP25</t>
+  </si>
+  <si>
+    <t>Edye presenta: Wibbly Pig está buscando su cubo favorito, tratando de encontrarlo se topa con muchas pistas.</t>
+  </si>
+  <si>
+    <t>Edye presenta: Wibbly Pig está buscando su cubo favorito, y no puede encontrarlo, por lo que los Pig Twins deciden ayudarlo. Pero están confundidos porque hay muchos rastros en la arena ¿Qué puede estar dejando huellas por todas partes?</t>
+  </si>
+  <si>
+    <t>EEWPIG125.mpg</t>
+  </si>
+  <si>
+    <t>EEWPIG125_land.jpg</t>
+  </si>
+  <si>
+    <t>EEWPIG126_SD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEWP6000000000000126</t>
+  </si>
+  <si>
+    <t>Las Aventuras de WibblyT01EP26</t>
+  </si>
+  <si>
+    <t>Las Aventuras de Wibbly T01 EP26</t>
+  </si>
+  <si>
+    <t>Edye presenta: Wibbly quiere jugar a las escondidas con sus amigos, pero¡no puede dejar de estornudar!</t>
+  </si>
+  <si>
+    <t>Edye presenta: Wibbly quiere jugar a las escondidas con sus amigos, pero hay un problema: ¡no puede dejar de estornudar! ¡No podrá esconderse en ningún lado porque se delatará! Intenta muchas formas diferentes de detener los estornudos, pero nada parece funcionar.</t>
+  </si>
+  <si>
+    <t>EEWPIG126.mpg</t>
+  </si>
+  <si>
+    <t>EEWPIG126_land.jpg</t>
+  </si>
+  <si>
+    <t>EEWPIG111_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEWP7000000000000111</t>
+  </si>
+  <si>
+    <t>Las Aventuras de Wibbly T01 EP11 HD</t>
+  </si>
+  <si>
+    <t>EEWPIG111.ts</t>
+  </si>
+  <si>
+    <t>EEWPIG112_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEWP7000000000000112</t>
+  </si>
+  <si>
+    <t>Las Aventuras de Wibbly T01 EP12 HD</t>
+  </si>
+  <si>
+    <t>EEWPIG112.ts</t>
+  </si>
+  <si>
+    <t>EEWPIG113_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEWP7000000000000113</t>
+  </si>
+  <si>
+    <t>Las Aventuras de Wibbly T01 EP13 HD</t>
+  </si>
+  <si>
+    <t>EEWPIG113.ts</t>
+  </si>
+  <si>
+    <t>EEWPIG114_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEWP7000000000000114</t>
+  </si>
+  <si>
+    <t>Las Aventuras de Wibbly T01 EP14 HD</t>
+  </si>
+  <si>
+    <t>EEWPIG114.ts</t>
+  </si>
+  <si>
+    <t>EEWPIG115_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEWP7000000000000115</t>
+  </si>
+  <si>
+    <t>Las Aventuras de Wibbly T01 EP15 HD</t>
+  </si>
+  <si>
+    <t>EEWPIG115.ts</t>
+  </si>
+  <si>
+    <t>EEWPIG116_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEWP7000000000000116</t>
+  </si>
+  <si>
+    <t>Las Aventuras de Wibbly T01 EP16 HD</t>
+  </si>
+  <si>
+    <t>EEWPIG116.ts</t>
+  </si>
+  <si>
+    <t>EEWPIG117_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEWP7000000000000117</t>
+  </si>
+  <si>
+    <t>Las Aventuras de Wibbly T01 EP17 HD</t>
+  </si>
+  <si>
+    <t>EEWPIG117.ts</t>
+  </si>
+  <si>
+    <t>EEWPIG118_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEWP7000000000000118</t>
+  </si>
+  <si>
+    <t>Las Aventuras de Wibbly T01 EP18 HD</t>
+  </si>
+  <si>
+    <t>EEWPIG118.ts</t>
+  </si>
+  <si>
+    <t>EEWPIG119_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEWP7000000000000119</t>
+  </si>
+  <si>
+    <t>Las Aventuras de Wibbly T01 EP19 HD</t>
+  </si>
+  <si>
+    <t>EEWPIG119.ts</t>
+  </si>
+  <si>
+    <t>EEWPIG120_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEWP7000000000000120</t>
+  </si>
+  <si>
+    <t>Las Aventuras de Wibbly T01 EP20 HD</t>
+  </si>
+  <si>
+    <t>EEWPIG120.ts</t>
+  </si>
+  <si>
+    <t>EEWPIG121_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEWP7000000000000121</t>
+  </si>
+  <si>
+    <t>Las Aventuras de Wibbly T01 EP21 HD</t>
+  </si>
+  <si>
+    <t>EEWPIG121.ts</t>
+  </si>
+  <si>
+    <t>EEWPIG122_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEWP7000000000000122</t>
+  </si>
+  <si>
+    <t>Las Aventuras de Wibbly T01 EP22 HD</t>
+  </si>
+  <si>
+    <t>EEWPIG122.ts</t>
+  </si>
+  <si>
+    <t>EEWPIG123_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEWP7000000000000123</t>
+  </si>
+  <si>
+    <t>Las Aventuras de Wibbly T01 EP23 HD</t>
+  </si>
+  <si>
+    <t>EEWPIG123.ts</t>
+  </si>
+  <si>
+    <t>EEWPIG124_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEWP7000000000000124</t>
+  </si>
+  <si>
+    <t>Las Aventuras de Wibbly T01 EP24 HD</t>
+  </si>
+  <si>
+    <t>EEWPIG124.ts</t>
+  </si>
+  <si>
+    <t>EEWPIG125_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEWP7000000000000125</t>
+  </si>
+  <si>
+    <t>Las Aventuras de Wibbly T01 EP25 HD</t>
+  </si>
+  <si>
+    <t>EEWPIG125.ts</t>
+  </si>
+  <si>
+    <t>EEWPIG126_HD_ADI.XML</t>
+  </si>
+  <si>
+    <t>EEWP7000000000000126</t>
+  </si>
+  <si>
+    <t>Las Aventuras de Wibbly T01 EP26 HD</t>
+  </si>
+  <si>
+    <t>EEWPIG126.ts</t>
   </si>
 </sst>
 </file>
@@ -1580,7 +1579,7 @@
         <v>81</v>
       </c>
       <c r="B2" s="7">
-        <v>44626</v>
+        <v>44623</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>43</v>
@@ -1632,13 +1631,13 @@
         <v>48</v>
       </c>
       <c r="T2" s="10">
-        <v>7.9861111111111122E-3</v>
+        <v>6.9328703703703696E-3</v>
       </c>
       <c r="U2" s="11">
-        <v>8.3333333333333332E-3</v>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="V2" s="3">
-        <v>2006</v>
+        <v>2009</v>
       </c>
       <c r="W2" s="9" t="s">
         <v>88</v>
@@ -1680,10 +1679,10 @@
         <v>92</v>
       </c>
       <c r="AJ2" s="9" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="AK2" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AL2" s="8"/>
       <c r="AM2" s="9" t="s">
@@ -1705,7 +1704,7 @@
         <v>55</v>
       </c>
       <c r="AS2" s="15">
-        <v>323128572</v>
+        <v>281577376</v>
       </c>
       <c r="AT2" s="9" t="s">
         <v>56</v>
@@ -1714,7 +1713,7 @@
         <v>57</v>
       </c>
       <c r="AV2" s="9" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="AW2" s="8"/>
       <c r="AX2" s="9" t="s">
@@ -1724,7 +1723,7 @@
         <v>58</v>
       </c>
       <c r="AZ2" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="BA2" s="8"/>
       <c r="BB2" s="9" t="s">
@@ -1740,15 +1739,15 @@
         <v>61</v>
       </c>
       <c r="BF2" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B3" s="7">
-        <v>44626</v>
+        <v>44623</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>43</v>
@@ -1769,13 +1768,13 @@
         <v>46</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J3" s="9" t="s">
         <v>83</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="L3" s="8"/>
       <c r="M3" s="9" t="s">
@@ -1785,28 +1784,28 @@
         <v>47</v>
       </c>
       <c r="O3" s="9" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="P3" s="9" t="s">
         <v>66</v>
       </c>
       <c r="Q3" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="R3" s="9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="S3" s="9" t="s">
         <v>48</v>
       </c>
       <c r="T3" s="10">
-        <v>7.9861111111111122E-3</v>
+        <v>6.9328703703703696E-3</v>
       </c>
       <c r="U3" s="11">
-        <v>8.3333333333333332E-3</v>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="V3" s="3">
-        <v>2006</v>
+        <v>2009</v>
       </c>
       <c r="W3" s="9" t="s">
         <v>88</v>
@@ -1848,10 +1847,10 @@
         <v>92</v>
       </c>
       <c r="AJ3" s="9" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="AK3" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AL3" s="8"/>
       <c r="AM3" s="9" t="s">
@@ -1873,7 +1872,7 @@
         <v>55</v>
       </c>
       <c r="AS3" s="15">
-        <v>324086620</v>
+        <v>281471344</v>
       </c>
       <c r="AT3" s="9" t="s">
         <v>56</v>
@@ -1882,7 +1881,7 @@
         <v>57</v>
       </c>
       <c r="AV3" s="9" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AW3" s="8"/>
       <c r="AX3" s="9" t="s">
@@ -1892,7 +1891,7 @@
         <v>58</v>
       </c>
       <c r="AZ3" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="BA3" s="8"/>
       <c r="BB3" s="9" t="s">
@@ -1908,15 +1907,15 @@
         <v>61</v>
       </c>
       <c r="BF3" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B4" s="7">
-        <v>44626</v>
+        <v>44623</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>43</v>
@@ -1937,13 +1936,13 @@
         <v>46</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="J4" s="9" t="s">
         <v>83</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="L4" s="8"/>
       <c r="M4" s="9" t="s">
@@ -1953,28 +1952,28 @@
         <v>47</v>
       </c>
       <c r="O4" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="P4" s="9" t="s">
         <v>67</v>
       </c>
       <c r="Q4" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="R4" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="S4" s="9" t="s">
         <v>48</v>
       </c>
       <c r="T4" s="10">
-        <v>7.9861111111111122E-3</v>
+        <v>6.9328703703703696E-3</v>
       </c>
       <c r="U4" s="11">
-        <v>8.3333333333333332E-3</v>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="V4" s="3">
-        <v>2006</v>
+        <v>2009</v>
       </c>
       <c r="W4" s="9" t="s">
         <v>88</v>
@@ -2016,10 +2015,10 @@
         <v>92</v>
       </c>
       <c r="AJ4" s="9" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="AK4" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AL4" s="8"/>
       <c r="AM4" s="9" t="s">
@@ -2041,7 +2040,7 @@
         <v>55</v>
       </c>
       <c r="AS4" s="15">
-        <v>323802740</v>
+        <v>281606140</v>
       </c>
       <c r="AT4" s="9" t="s">
         <v>56</v>
@@ -2050,7 +2049,7 @@
         <v>57</v>
       </c>
       <c r="AV4" s="9" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="AW4" s="8"/>
       <c r="AX4" s="9" t="s">
@@ -2060,7 +2059,7 @@
         <v>58</v>
       </c>
       <c r="AZ4" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="BA4" s="8"/>
       <c r="BB4" s="9" t="s">
@@ -2076,15 +2075,15 @@
         <v>61</v>
       </c>
       <c r="BF4" s="9" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B5" s="7">
-        <v>44626</v>
+        <v>44623</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>43</v>
@@ -2105,13 +2104,13 @@
         <v>46</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="J5" s="9" t="s">
         <v>83</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="L5" s="8"/>
       <c r="M5" s="9" t="s">
@@ -2121,28 +2120,28 @@
         <v>47</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="P5" s="9" t="s">
         <v>68</v>
       </c>
       <c r="Q5" s="9" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="R5" s="9" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="S5" s="9" t="s">
         <v>48</v>
       </c>
       <c r="T5" s="10">
-        <v>7.9861111111111122E-3</v>
+        <v>6.9328703703703696E-3</v>
       </c>
       <c r="U5" s="11">
-        <v>8.3333333333333332E-3</v>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="V5" s="3">
-        <v>2006</v>
+        <v>2009</v>
       </c>
       <c r="W5" s="9" t="s">
         <v>88</v>
@@ -2184,10 +2183,10 @@
         <v>92</v>
       </c>
       <c r="AJ5" s="9" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="AK5" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AL5" s="8"/>
       <c r="AM5" s="9" t="s">
@@ -2209,7 +2208,7 @@
         <v>55</v>
       </c>
       <c r="AS5" s="15">
-        <v>324086620</v>
+        <v>281428292</v>
       </c>
       <c r="AT5" s="9" t="s">
         <v>56</v>
@@ -2218,7 +2217,7 @@
         <v>57</v>
       </c>
       <c r="AV5" s="9" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="AW5" s="8"/>
       <c r="AX5" s="9" t="s">
@@ -2228,7 +2227,7 @@
         <v>58</v>
       </c>
       <c r="AZ5" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="BA5" s="8"/>
       <c r="BB5" s="9" t="s">
@@ -2244,15 +2243,15 @@
         <v>61</v>
       </c>
       <c r="BF5" s="9" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B6" s="7">
-        <v>44626</v>
+        <v>44623</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>43</v>
@@ -2273,13 +2272,13 @@
         <v>46</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="J6" s="9" t="s">
         <v>83</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="L6" s="8"/>
       <c r="M6" s="9" t="s">
@@ -2289,28 +2288,28 @@
         <v>47</v>
       </c>
       <c r="O6" s="9" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="P6" s="9" t="s">
         <v>69</v>
       </c>
       <c r="Q6" s="9" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="R6" s="9" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="S6" s="9" t="s">
         <v>48</v>
       </c>
       <c r="T6" s="10">
-        <v>7.9861111111111122E-3</v>
+        <v>6.9328703703703696E-3</v>
       </c>
       <c r="U6" s="11">
-        <v>8.3333333333333332E-3</v>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="V6" s="3">
-        <v>2006</v>
+        <v>2009</v>
       </c>
       <c r="W6" s="9" t="s">
         <v>88</v>
@@ -2352,10 +2351,10 @@
         <v>92</v>
       </c>
       <c r="AJ6" s="9" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="AK6" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AL6" s="8"/>
       <c r="AM6" s="9" t="s">
@@ -2377,7 +2376,7 @@
         <v>55</v>
       </c>
       <c r="AS6" s="15">
-        <v>324101096</v>
+        <v>281577376</v>
       </c>
       <c r="AT6" s="9" t="s">
         <v>56</v>
@@ -2386,7 +2385,7 @@
         <v>57</v>
       </c>
       <c r="AV6" s="9" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="AW6" s="8"/>
       <c r="AX6" s="9" t="s">
@@ -2396,7 +2395,7 @@
         <v>58</v>
       </c>
       <c r="AZ6" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="BA6" s="8"/>
       <c r="BB6" s="9" t="s">
@@ -2412,15 +2411,15 @@
         <v>61</v>
       </c>
       <c r="BF6" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B7" s="7">
-        <v>44626</v>
+        <v>44623</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>43</v>
@@ -2441,13 +2440,13 @@
         <v>46</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="J7" s="9" t="s">
         <v>83</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L7" s="8"/>
       <c r="M7" s="9" t="s">
@@ -2457,28 +2456,28 @@
         <v>47</v>
       </c>
       <c r="O7" s="9" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="P7" s="9" t="s">
         <v>70</v>
       </c>
       <c r="Q7" s="9" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="R7" s="9" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="S7" s="9" t="s">
         <v>48</v>
       </c>
       <c r="T7" s="10">
-        <v>7.9861111111111122E-3</v>
+        <v>6.9328703703703696E-3</v>
       </c>
       <c r="U7" s="11">
-        <v>8.3333333333333332E-3</v>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="V7" s="3">
-        <v>2006</v>
+        <v>2009</v>
       </c>
       <c r="W7" s="9" t="s">
         <v>88</v>
@@ -2520,10 +2519,10 @@
         <v>92</v>
       </c>
       <c r="AJ7" s="9" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="AK7" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AL7" s="8"/>
       <c r="AM7" s="9" t="s">
@@ -2545,7 +2544,7 @@
         <v>55</v>
       </c>
       <c r="AS7" s="15">
-        <v>324101096</v>
+        <v>281531504</v>
       </c>
       <c r="AT7" s="9" t="s">
         <v>56</v>
@@ -2554,7 +2553,7 @@
         <v>57</v>
       </c>
       <c r="AV7" s="9" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="AW7" s="8"/>
       <c r="AX7" s="9" t="s">
@@ -2564,7 +2563,7 @@
         <v>58</v>
       </c>
       <c r="AZ7" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="BA7" s="8"/>
       <c r="BB7" s="9" t="s">
@@ -2580,15 +2579,15 @@
         <v>61</v>
       </c>
       <c r="BF7" s="9" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B8" s="7">
-        <v>44626</v>
+        <v>44623</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>43</v>
@@ -2609,13 +2608,13 @@
         <v>46</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="J8" s="9" t="s">
         <v>83</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="L8" s="8"/>
       <c r="M8" s="9" t="s">
@@ -2625,13 +2624,13 @@
         <v>47</v>
       </c>
       <c r="O8" s="9" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="P8" s="9" t="s">
         <v>71</v>
       </c>
       <c r="Q8" s="9" t="s">
-        <v>141</v>
+        <v>110</v>
       </c>
       <c r="R8" s="9" t="s">
         <v>142</v>
@@ -2640,13 +2639,13 @@
         <v>48</v>
       </c>
       <c r="T8" s="10">
-        <v>7.9861111111111122E-3</v>
+        <v>6.9328703703703696E-3</v>
       </c>
       <c r="U8" s="11">
-        <v>8.3333333333333332E-3</v>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="V8" s="3">
-        <v>2006</v>
+        <v>2009</v>
       </c>
       <c r="W8" s="9" t="s">
         <v>88</v>
@@ -2688,10 +2687,10 @@
         <v>92</v>
       </c>
       <c r="AJ8" s="9" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="AK8" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AL8" s="8"/>
       <c r="AM8" s="9" t="s">
@@ -2713,7 +2712,7 @@
         <v>55</v>
       </c>
       <c r="AS8" s="15">
-        <v>324101096</v>
+        <v>281247436</v>
       </c>
       <c r="AT8" s="9" t="s">
         <v>56</v>
@@ -2732,7 +2731,7 @@
         <v>58</v>
       </c>
       <c r="AZ8" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="BA8" s="8"/>
       <c r="BB8" s="9" t="s">
@@ -2756,7 +2755,7 @@
         <v>145</v>
       </c>
       <c r="B9" s="7">
-        <v>44626</v>
+        <v>44623</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>43</v>
@@ -2808,13 +2807,13 @@
         <v>48</v>
       </c>
       <c r="T9" s="10">
-        <v>7.9861111111111122E-3</v>
+        <v>6.9328703703703696E-3</v>
       </c>
       <c r="U9" s="11">
-        <v>8.3333333333333332E-3</v>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="V9" s="3">
-        <v>2006</v>
+        <v>2009</v>
       </c>
       <c r="W9" s="9" t="s">
         <v>88</v>
@@ -2856,10 +2855,10 @@
         <v>92</v>
       </c>
       <c r="AJ9" s="9" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="AK9" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AL9" s="8"/>
       <c r="AM9" s="9" t="s">
@@ -2881,7 +2880,7 @@
         <v>55</v>
       </c>
       <c r="AS9" s="15">
-        <v>324118204</v>
+        <v>281623248</v>
       </c>
       <c r="AT9" s="9" t="s">
         <v>56</v>
@@ -2900,7 +2899,7 @@
         <v>58</v>
       </c>
       <c r="AZ9" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="BA9" s="8"/>
       <c r="BB9" s="9" t="s">
@@ -2924,7 +2923,7 @@
         <v>153</v>
       </c>
       <c r="B10" s="7">
-        <v>44626</v>
+        <v>44623</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>43</v>
@@ -2976,13 +2975,13 @@
         <v>48</v>
       </c>
       <c r="T10" s="10">
-        <v>7.9861111111111122E-3</v>
+        <v>6.9328703703703696E-3</v>
       </c>
       <c r="U10" s="11">
-        <v>8.3333333333333332E-3</v>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="V10" s="3">
-        <v>2006</v>
+        <v>2009</v>
       </c>
       <c r="W10" s="9" t="s">
         <v>88</v>
@@ -3024,10 +3023,10 @@
         <v>92</v>
       </c>
       <c r="AJ10" s="9" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="AK10" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AL10" s="8"/>
       <c r="AM10" s="9" t="s">
@@ -3049,7 +3048,7 @@
         <v>55</v>
       </c>
       <c r="AS10" s="15">
-        <v>324118204</v>
+        <v>281545792</v>
       </c>
       <c r="AT10" s="9" t="s">
         <v>56</v>
@@ -3068,7 +3067,7 @@
         <v>58</v>
       </c>
       <c r="AZ10" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="BA10" s="8"/>
       <c r="BB10" s="9" t="s">
@@ -3092,7 +3091,7 @@
         <v>161</v>
       </c>
       <c r="B11" s="7">
-        <v>44626</v>
+        <v>44623</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>43</v>
@@ -3144,13 +3143,13 @@
         <v>48</v>
       </c>
       <c r="T11" s="10">
-        <v>7.9861111111111122E-3</v>
+        <v>6.9328703703703696E-3</v>
       </c>
       <c r="U11" s="11">
-        <v>8.3333333333333332E-3</v>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="V11" s="3">
-        <v>2006</v>
+        <v>2009</v>
       </c>
       <c r="W11" s="9" t="s">
         <v>88</v>
@@ -3192,10 +3191,10 @@
         <v>92</v>
       </c>
       <c r="AJ11" s="9" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="AK11" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AL11" s="8"/>
       <c r="AM11" s="9" t="s">
@@ -3217,7 +3216,7 @@
         <v>55</v>
       </c>
       <c r="AS11" s="15">
-        <v>324132492</v>
+        <v>281591852</v>
       </c>
       <c r="AT11" s="9" t="s">
         <v>56</v>
@@ -3236,7 +3235,7 @@
         <v>58</v>
       </c>
       <c r="AZ11" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="BA11" s="8"/>
       <c r="BB11" s="9" t="s">
@@ -3260,7 +3259,7 @@
         <v>169</v>
       </c>
       <c r="B12" s="7">
-        <v>44626</v>
+        <v>44623</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>43</v>
@@ -3312,13 +3311,13 @@
         <v>48</v>
       </c>
       <c r="T12" s="10">
-        <v>7.9861111111111122E-3</v>
+        <v>6.9328703703703696E-3</v>
       </c>
       <c r="U12" s="11">
-        <v>8.3333333333333332E-3</v>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="V12" s="3">
-        <v>2006</v>
+        <v>2009</v>
       </c>
       <c r="W12" s="9" t="s">
         <v>88</v>
@@ -3360,10 +3359,10 @@
         <v>92</v>
       </c>
       <c r="AJ12" s="9" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="AK12" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AL12" s="8"/>
       <c r="AM12" s="9" t="s">
@@ -3385,7 +3384,7 @@
         <v>55</v>
       </c>
       <c r="AS12" s="9">
-        <v>324118204</v>
+        <v>281758232</v>
       </c>
       <c r="AT12" s="9" t="s">
         <v>56</v>
@@ -3404,7 +3403,7 @@
         <v>58</v>
       </c>
       <c r="AZ12" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="BA12" s="8"/>
       <c r="BB12" s="9" t="s">
@@ -3428,7 +3427,7 @@
         <v>177</v>
       </c>
       <c r="B13" s="7">
-        <v>44626</v>
+        <v>44623</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>43</v>
@@ -3480,13 +3479,13 @@
         <v>48</v>
       </c>
       <c r="T13" s="10">
-        <v>7.9861111111111122E-3</v>
+        <v>6.9328703703703696E-3</v>
       </c>
       <c r="U13" s="11">
-        <v>8.3333333333333332E-3</v>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="V13" s="3">
-        <v>2006</v>
+        <v>2009</v>
       </c>
       <c r="W13" s="9" t="s">
         <v>88</v>
@@ -3528,10 +3527,10 @@
         <v>92</v>
       </c>
       <c r="AJ13" s="9" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="AK13" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AL13" s="8"/>
       <c r="AM13" s="9" t="s">
@@ -3553,7 +3552,7 @@
         <v>55</v>
       </c>
       <c r="AS13" s="9">
-        <v>324101096</v>
+        <v>281442580</v>
       </c>
       <c r="AT13" s="9" t="s">
         <v>56</v>
@@ -3572,7 +3571,7 @@
         <v>58</v>
       </c>
       <c r="AZ13" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="BA13" s="8"/>
       <c r="BB13" s="9" t="s">
@@ -3596,7 +3595,7 @@
         <v>185</v>
       </c>
       <c r="B14" s="7">
-        <v>44626</v>
+        <v>44623</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>43</v>
@@ -3648,13 +3647,13 @@
         <v>48</v>
       </c>
       <c r="T14" s="10">
-        <v>7.9861111111111122E-3</v>
+        <v>6.9328703703703696E-3</v>
       </c>
       <c r="U14" s="11">
-        <v>8.3333333333333332E-3</v>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="V14" s="3">
-        <v>2006</v>
+        <v>2009</v>
       </c>
       <c r="W14" s="9" t="s">
         <v>88</v>
@@ -3696,10 +3695,10 @@
         <v>92</v>
       </c>
       <c r="AJ14" s="9" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="AK14" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AL14" s="8"/>
       <c r="AM14" s="9" t="s">
@@ -3721,7 +3720,7 @@
         <v>55</v>
       </c>
       <c r="AS14" s="9">
-        <v>324118204</v>
+        <v>281442580</v>
       </c>
       <c r="AT14" s="9" t="s">
         <v>56</v>
@@ -3740,7 +3739,7 @@
         <v>58</v>
       </c>
       <c r="AZ14" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="BA14" s="8"/>
       <c r="BB14" s="9" t="s">
@@ -3764,7 +3763,7 @@
         <v>193</v>
       </c>
       <c r="B15" s="7">
-        <v>44626</v>
+        <v>44623</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>43</v>
@@ -3816,13 +3815,13 @@
         <v>48</v>
       </c>
       <c r="T15" s="10">
-        <v>7.9861111111111122E-3</v>
+        <v>6.9328703703703696E-3</v>
       </c>
       <c r="U15" s="11">
-        <v>8.3333333333333332E-3</v>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="V15" s="3">
-        <v>2006</v>
+        <v>2009</v>
       </c>
       <c r="W15" s="9" t="s">
         <v>88</v>
@@ -3864,10 +3863,10 @@
         <v>92</v>
       </c>
       <c r="AJ15" s="9" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="AK15" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AL15" s="8"/>
       <c r="AM15" s="9" t="s">
@@ -3889,7 +3888,7 @@
         <v>55</v>
       </c>
       <c r="AS15" s="9">
-        <v>324101096</v>
+        <v>281442580</v>
       </c>
       <c r="AT15" s="9" t="s">
         <v>56</v>
@@ -3908,7 +3907,7 @@
         <v>58</v>
       </c>
       <c r="AZ15" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="BA15" s="8"/>
       <c r="BB15" s="9" t="s">
@@ -3932,7 +3931,7 @@
         <v>201</v>
       </c>
       <c r="B16" s="7">
-        <v>44626</v>
+        <v>44623</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>43</v>
@@ -3984,13 +3983,13 @@
         <v>48</v>
       </c>
       <c r="T16" s="10">
-        <v>7.9861111111111122E-3</v>
+        <v>6.9328703703703696E-3</v>
       </c>
       <c r="U16" s="11">
-        <v>8.3333333333333332E-3</v>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="V16" s="3">
-        <v>2006</v>
+        <v>2009</v>
       </c>
       <c r="W16" s="9" t="s">
         <v>88</v>
@@ -4032,10 +4031,10 @@
         <v>92</v>
       </c>
       <c r="AJ16" s="9" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="AK16" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AL16" s="8"/>
       <c r="AM16" s="9" t="s">
@@ -4057,7 +4056,7 @@
         <v>55</v>
       </c>
       <c r="AS16" s="9">
-        <v>324118204</v>
+        <v>281396708</v>
       </c>
       <c r="AT16" s="9" t="s">
         <v>56</v>
@@ -4076,7 +4075,7 @@
         <v>58</v>
       </c>
       <c r="AZ16" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="BA16" s="8"/>
       <c r="BB16" s="9" t="s">
@@ -4100,7 +4099,7 @@
         <v>209</v>
       </c>
       <c r="B17" s="7">
-        <v>44626</v>
+        <v>44623</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>43</v>
@@ -4152,13 +4151,13 @@
         <v>48</v>
       </c>
       <c r="T17" s="10">
-        <v>7.9861111111111122E-3</v>
+        <v>6.9328703703703696E-3</v>
       </c>
       <c r="U17" s="11">
-        <v>8.3333333333333332E-3</v>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="V17" s="3">
-        <v>2006</v>
+        <v>2009</v>
       </c>
       <c r="W17" s="9" t="s">
         <v>88</v>
@@ -4200,10 +4199,10 @@
         <v>92</v>
       </c>
       <c r="AJ17" s="9" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="AK17" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AL17" s="8"/>
       <c r="AM17" s="9" t="s">
@@ -4225,7 +4224,7 @@
         <v>55</v>
       </c>
       <c r="AS17" s="9">
-        <v>324118204</v>
+        <v>281442580</v>
       </c>
       <c r="AT17" s="9" t="s">
         <v>56</v>
@@ -4244,7 +4243,7 @@
         <v>58</v>
       </c>
       <c r="AZ17" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="BA17" s="8"/>
       <c r="BB17" s="9" t="s">
@@ -4873,7 +4872,7 @@
   <dimension ref="A1:BF27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:BF17"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5096,7 +5095,7 @@
         <v>217</v>
       </c>
       <c r="B2" s="12">
-        <v>44626</v>
+        <v>44623</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>43</v>
@@ -5148,13 +5147,13 @@
         <v>48</v>
       </c>
       <c r="T2" s="10">
-        <v>7.9861111111111122E-3</v>
+        <v>6.9328703703703696E-3</v>
       </c>
       <c r="U2" s="11">
-        <v>8.3333333333333332E-3</v>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="V2" s="9">
-        <v>2006</v>
+        <v>2009</v>
       </c>
       <c r="W2" s="9" t="s">
         <v>88</v>
@@ -5196,10 +5195,10 @@
         <v>92</v>
       </c>
       <c r="AJ2" s="9" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="AK2" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AL2" s="8"/>
       <c r="AM2" s="9" t="s">
@@ -5221,7 +5220,7 @@
         <v>55</v>
       </c>
       <c r="AS2" s="15">
-        <v>646193600</v>
+        <v>563097224</v>
       </c>
       <c r="AT2" s="9" t="s">
         <v>55</v>
@@ -5240,7 +5239,7 @@
         <v>58</v>
       </c>
       <c r="AZ2" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="BA2" s="8"/>
       <c r="BB2" s="9" t="s">
@@ -5256,7 +5255,7 @@
         <v>61</v>
       </c>
       <c r="BF2" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:58" x14ac:dyDescent="0.25">
@@ -5264,7 +5263,7 @@
         <v>221</v>
       </c>
       <c r="B3" s="12">
-        <v>44626</v>
+        <v>44623</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>43</v>
@@ -5291,7 +5290,7 @@
         <v>83</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="L3" s="8"/>
       <c r="M3" s="9" t="s">
@@ -5307,22 +5306,22 @@
         <v>66</v>
       </c>
       <c r="Q3" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="R3" s="9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="S3" s="9" t="s">
         <v>48</v>
       </c>
       <c r="T3" s="10">
-        <v>7.9861111111111122E-3</v>
+        <v>6.9328703703703696E-3</v>
       </c>
       <c r="U3" s="11">
-        <v>8.3333333333333332E-3</v>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="V3" s="9">
-        <v>2006</v>
+        <v>2009</v>
       </c>
       <c r="W3" s="9" t="s">
         <v>88</v>
@@ -5364,10 +5363,10 @@
         <v>92</v>
       </c>
       <c r="AJ3" s="9" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="AK3" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AL3" s="8"/>
       <c r="AM3" s="9" t="s">
@@ -5389,7 +5388,7 @@
         <v>55</v>
       </c>
       <c r="AS3" s="15">
-        <v>648115712</v>
+        <v>562884972</v>
       </c>
       <c r="AT3" s="9" t="s">
         <v>55</v>
@@ -5408,7 +5407,7 @@
         <v>58</v>
       </c>
       <c r="AZ3" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="BA3" s="8"/>
       <c r="BB3" s="9" t="s">
@@ -5424,7 +5423,7 @@
         <v>61</v>
       </c>
       <c r="BF3" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:58" x14ac:dyDescent="0.25">
@@ -5432,7 +5431,7 @@
         <v>225</v>
       </c>
       <c r="B4" s="12">
-        <v>44626</v>
+        <v>44623</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>43</v>
@@ -5459,7 +5458,7 @@
         <v>83</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="L4" s="8"/>
       <c r="M4" s="9" t="s">
@@ -5475,22 +5474,22 @@
         <v>67</v>
       </c>
       <c r="Q4" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="R4" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="S4" s="9" t="s">
         <v>48</v>
       </c>
       <c r="T4" s="10">
-        <v>7.9861111111111122E-3</v>
+        <v>6.9328703703703696E-3</v>
       </c>
       <c r="U4" s="11">
-        <v>8.3333333333333332E-3</v>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="V4" s="9">
-        <v>2006</v>
+        <v>2009</v>
       </c>
       <c r="W4" s="9" t="s">
         <v>88</v>
@@ -5532,10 +5531,10 @@
         <v>92</v>
       </c>
       <c r="AJ4" s="9" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="AK4" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AL4" s="8"/>
       <c r="AM4" s="9" t="s">
@@ -5557,7 +5556,7 @@
         <v>55</v>
       </c>
       <c r="AS4" s="15">
-        <v>647547764</v>
+        <v>563154564</v>
       </c>
       <c r="AT4" s="9" t="s">
         <v>55</v>
@@ -5576,7 +5575,7 @@
         <v>58</v>
       </c>
       <c r="AZ4" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="BA4" s="8"/>
       <c r="BB4" s="9" t="s">
@@ -5592,7 +5591,7 @@
         <v>61</v>
       </c>
       <c r="BF4" s="9" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:58" x14ac:dyDescent="0.25">
@@ -5600,7 +5599,7 @@
         <v>229</v>
       </c>
       <c r="B5" s="12">
-        <v>44626</v>
+        <v>44623</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>43</v>
@@ -5627,7 +5626,7 @@
         <v>83</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="L5" s="8"/>
       <c r="M5" s="9" t="s">
@@ -5643,22 +5642,22 @@
         <v>68</v>
       </c>
       <c r="Q5" s="9" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="R5" s="9" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="S5" s="9" t="s">
         <v>48</v>
       </c>
       <c r="T5" s="10">
-        <v>7.9861111111111122E-3</v>
+        <v>6.9328703703703696E-3</v>
       </c>
       <c r="U5" s="11">
-        <v>8.3333333333333332E-3</v>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="V5" s="9">
-        <v>2006</v>
+        <v>2009</v>
       </c>
       <c r="W5" s="9" t="s">
         <v>88</v>
@@ -5700,10 +5699,10 @@
         <v>92</v>
       </c>
       <c r="AJ5" s="9" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="AK5" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AL5" s="8"/>
       <c r="AM5" s="9" t="s">
@@ -5725,7 +5724,7 @@
         <v>55</v>
       </c>
       <c r="AS5" s="15">
-        <v>648115712</v>
+        <v>562793040</v>
       </c>
       <c r="AT5" s="9" t="s">
         <v>55</v>
@@ -5744,7 +5743,7 @@
         <v>58</v>
       </c>
       <c r="AZ5" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="BA5" s="8"/>
       <c r="BB5" s="9" t="s">
@@ -5760,7 +5759,7 @@
         <v>61</v>
       </c>
       <c r="BF5" s="9" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:58" x14ac:dyDescent="0.25">
@@ -5768,7 +5767,7 @@
         <v>233</v>
       </c>
       <c r="B6" s="12">
-        <v>44626</v>
+        <v>44623</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>43</v>
@@ -5795,7 +5794,7 @@
         <v>83</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="L6" s="8"/>
       <c r="M6" s="9" t="s">
@@ -5811,22 +5810,22 @@
         <v>69</v>
       </c>
       <c r="Q6" s="9" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="R6" s="9" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="S6" s="9" t="s">
         <v>48</v>
       </c>
       <c r="T6" s="10">
-        <v>7.9861111111111122E-3</v>
+        <v>6.9328703703703696E-3</v>
       </c>
       <c r="U6" s="11">
-        <v>8.3333333333333332E-3</v>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="V6" s="9">
-        <v>2006</v>
+        <v>2009</v>
       </c>
       <c r="W6" s="9" t="s">
         <v>88</v>
@@ -5868,10 +5867,10 @@
         <v>92</v>
       </c>
       <c r="AJ6" s="9" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="AK6" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AL6" s="8"/>
       <c r="AM6" s="9" t="s">
@@ -5893,7 +5892,7 @@
         <v>55</v>
       </c>
       <c r="AS6" s="15">
-        <v>648144288</v>
+        <v>563097224</v>
       </c>
       <c r="AT6" s="9" t="s">
         <v>55</v>
@@ -5912,7 +5911,7 @@
         <v>58</v>
       </c>
       <c r="AZ6" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="BA6" s="8"/>
       <c r="BB6" s="9" t="s">
@@ -5928,7 +5927,7 @@
         <v>61</v>
       </c>
       <c r="BF6" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:58" x14ac:dyDescent="0.25">
@@ -5936,7 +5935,7 @@
         <v>237</v>
       </c>
       <c r="B7" s="12">
-        <v>44626</v>
+        <v>44623</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>43</v>
@@ -5963,7 +5962,7 @@
         <v>83</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L7" s="8"/>
       <c r="M7" s="9" t="s">
@@ -5979,22 +5978,22 @@
         <v>70</v>
       </c>
       <c r="Q7" s="9" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="R7" s="9" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="S7" s="9" t="s">
         <v>48</v>
       </c>
       <c r="T7" s="10">
-        <v>7.9861111111111122E-3</v>
+        <v>6.9328703703703696E-3</v>
       </c>
       <c r="U7" s="11">
-        <v>8.3333333333333332E-3</v>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="V7" s="9">
-        <v>2006</v>
+        <v>2009</v>
       </c>
       <c r="W7" s="9" t="s">
         <v>88</v>
@@ -6036,10 +6035,10 @@
         <v>92</v>
       </c>
       <c r="AJ7" s="9" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="AK7" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AL7" s="8"/>
       <c r="AM7" s="9" t="s">
@@ -6061,7 +6060,7 @@
         <v>55</v>
       </c>
       <c r="AS7" s="15">
-        <v>648144288</v>
+        <v>563005480</v>
       </c>
       <c r="AT7" s="9" t="s">
         <v>55</v>
@@ -6080,7 +6079,7 @@
         <v>58</v>
       </c>
       <c r="AZ7" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="BA7" s="8"/>
       <c r="BB7" s="9" t="s">
@@ -6096,7 +6095,7 @@
         <v>61</v>
       </c>
       <c r="BF7" s="9" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:58" x14ac:dyDescent="0.25">
@@ -6104,7 +6103,7 @@
         <v>241</v>
       </c>
       <c r="B8" s="12">
-        <v>44626</v>
+        <v>44623</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>43</v>
@@ -6131,7 +6130,7 @@
         <v>83</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="L8" s="8"/>
       <c r="M8" s="9" t="s">
@@ -6147,7 +6146,7 @@
         <v>71</v>
       </c>
       <c r="Q8" s="9" t="s">
-        <v>141</v>
+        <v>110</v>
       </c>
       <c r="R8" s="9" t="s">
         <v>142</v>
@@ -6156,13 +6155,13 @@
         <v>48</v>
       </c>
       <c r="T8" s="10">
-        <v>7.9861111111111122E-3</v>
+        <v>6.9328703703703696E-3</v>
       </c>
       <c r="U8" s="11">
-        <v>8.3333333333333332E-3</v>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="V8" s="9">
-        <v>2006</v>
+        <v>2009</v>
       </c>
       <c r="W8" s="9" t="s">
         <v>88</v>
@@ -6204,10 +6203,10 @@
         <v>92</v>
       </c>
       <c r="AJ8" s="9" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="AK8" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AL8" s="8"/>
       <c r="AM8" s="9" t="s">
@@ -6229,7 +6228,7 @@
         <v>55</v>
       </c>
       <c r="AS8" s="15">
-        <v>648144288</v>
+        <v>562437344</v>
       </c>
       <c r="AT8" s="9" t="s">
         <v>55</v>
@@ -6248,7 +6247,7 @@
         <v>58</v>
       </c>
       <c r="AZ8" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="BA8" s="8"/>
       <c r="BB8" s="9" t="s">
@@ -6272,7 +6271,7 @@
         <v>245</v>
       </c>
       <c r="B9" s="12">
-        <v>44626</v>
+        <v>44623</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>43</v>
@@ -6324,13 +6323,13 @@
         <v>48</v>
       </c>
       <c r="T9" s="10">
-        <v>7.9861111111111122E-3</v>
+        <v>6.9328703703703696E-3</v>
       </c>
       <c r="U9" s="11">
-        <v>8.3333333333333332E-3</v>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="V9" s="9">
-        <v>2006</v>
+        <v>2009</v>
       </c>
       <c r="W9" s="9" t="s">
         <v>88</v>
@@ -6372,10 +6371,10 @@
         <v>92</v>
       </c>
       <c r="AJ9" s="9" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="AK9" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AL9" s="8"/>
       <c r="AM9" s="9" t="s">
@@ -6397,7 +6396,7 @@
         <v>55</v>
       </c>
       <c r="AS9" s="15">
-        <v>648173052</v>
+        <v>563183328</v>
       </c>
       <c r="AT9" s="9" t="s">
         <v>55</v>
@@ -6416,7 +6415,7 @@
         <v>58</v>
       </c>
       <c r="AZ9" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="BA9" s="8"/>
       <c r="BB9" s="9" t="s">
@@ -6440,7 +6439,7 @@
         <v>249</v>
       </c>
       <c r="B10" s="12">
-        <v>44626</v>
+        <v>44623</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>43</v>
@@ -6492,13 +6491,13 @@
         <v>48</v>
       </c>
       <c r="T10" s="10">
-        <v>7.9861111111111122E-3</v>
+        <v>6.9328703703703696E-3</v>
       </c>
       <c r="U10" s="11">
-        <v>8.3333333333333332E-3</v>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="V10" s="9">
-        <v>2006</v>
+        <v>2009</v>
       </c>
       <c r="W10" s="9" t="s">
         <v>88</v>
@@ -6540,10 +6539,10 @@
         <v>92</v>
       </c>
       <c r="AJ10" s="9" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="AK10" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AL10" s="8"/>
       <c r="AM10" s="9" t="s">
@@ -6565,7 +6564,7 @@
         <v>55</v>
       </c>
       <c r="AS10" s="15">
-        <v>648173052</v>
+        <v>563034056</v>
       </c>
       <c r="AT10" s="9" t="s">
         <v>55</v>
@@ -6584,7 +6583,7 @@
         <v>58</v>
       </c>
       <c r="AZ10" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="BA10" s="8"/>
       <c r="BB10" s="9" t="s">
@@ -6608,7 +6607,7 @@
         <v>253</v>
       </c>
       <c r="B11" s="12">
-        <v>44626</v>
+        <v>44623</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>43</v>
@@ -6660,13 +6659,13 @@
         <v>48</v>
       </c>
       <c r="T11" s="10">
-        <v>7.9861111111111122E-3</v>
+        <v>6.9328703703703696E-3</v>
       </c>
       <c r="U11" s="11">
-        <v>8.3333333333333332E-3</v>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="V11" s="9">
-        <v>2006</v>
+        <v>2009</v>
       </c>
       <c r="W11" s="9" t="s">
         <v>88</v>
@@ -6708,10 +6707,10 @@
         <v>92</v>
       </c>
       <c r="AJ11" s="9" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="AK11" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AL11" s="8"/>
       <c r="AM11" s="9" t="s">
@@ -6733,7 +6732,7 @@
         <v>55</v>
       </c>
       <c r="AS11" s="9">
-        <v>648207456</v>
+        <v>563125800</v>
       </c>
       <c r="AT11" s="9" t="s">
         <v>55</v>
@@ -6752,7 +6751,7 @@
         <v>58</v>
       </c>
       <c r="AZ11" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="BA11" s="8"/>
       <c r="BB11" s="9" t="s">
@@ -6776,7 +6775,7 @@
         <v>257</v>
       </c>
       <c r="B12" s="12">
-        <v>44626</v>
+        <v>44623</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>43</v>
@@ -6828,13 +6827,13 @@
         <v>48</v>
       </c>
       <c r="T12" s="10">
-        <v>7.9861111111111122E-3</v>
+        <v>6.9328703703703696E-3</v>
       </c>
       <c r="U12" s="11">
-        <v>8.3333333333333332E-3</v>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="V12" s="9">
-        <v>2006</v>
+        <v>2009</v>
       </c>
       <c r="W12" s="9" t="s">
         <v>88</v>
@@ -6876,10 +6875,10 @@
         <v>92</v>
       </c>
       <c r="AJ12" s="9" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="AK12" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AL12" s="8"/>
       <c r="AM12" s="9" t="s">
@@ -6901,7 +6900,7 @@
         <v>55</v>
       </c>
       <c r="AS12" s="9">
-        <v>648173052</v>
+        <v>563452920</v>
       </c>
       <c r="AT12" s="9" t="s">
         <v>55</v>
@@ -6920,7 +6919,7 @@
         <v>58</v>
       </c>
       <c r="AZ12" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="BA12" s="8"/>
       <c r="BB12" s="9" t="s">
@@ -6944,7 +6943,7 @@
         <v>261</v>
       </c>
       <c r="B13" s="12">
-        <v>44626</v>
+        <v>44623</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>43</v>
@@ -6996,13 +6995,13 @@
         <v>48</v>
       </c>
       <c r="T13" s="10">
-        <v>7.9861111111111122E-3</v>
+        <v>6.9328703703703696E-3</v>
       </c>
       <c r="U13" s="11">
-        <v>8.3333333333333332E-3</v>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="V13" s="9">
-        <v>2006</v>
+        <v>2009</v>
       </c>
       <c r="W13" s="9" t="s">
         <v>88</v>
@@ -7044,10 +7043,10 @@
         <v>92</v>
       </c>
       <c r="AJ13" s="9" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="AK13" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AL13" s="8"/>
       <c r="AM13" s="9" t="s">
@@ -7069,7 +7068,7 @@
         <v>55</v>
       </c>
       <c r="AS13" s="9">
-        <v>648144288</v>
+        <v>562827444</v>
       </c>
       <c r="AT13" s="9" t="s">
         <v>55</v>
@@ -7088,7 +7087,7 @@
         <v>58</v>
       </c>
       <c r="AZ13" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="BA13" s="8"/>
       <c r="BB13" s="9" t="s">
@@ -7112,7 +7111,7 @@
         <v>265</v>
       </c>
       <c r="B14" s="12">
-        <v>44626</v>
+        <v>44623</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>43</v>
@@ -7164,13 +7163,13 @@
         <v>48</v>
       </c>
       <c r="T14" s="10">
-        <v>7.9861111111111122E-3</v>
+        <v>6.9328703703703696E-3</v>
       </c>
       <c r="U14" s="11">
-        <v>8.3333333333333332E-3</v>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="V14" s="9">
-        <v>2006</v>
+        <v>2009</v>
       </c>
       <c r="W14" s="9" t="s">
         <v>88</v>
@@ -7212,10 +7211,10 @@
         <v>92</v>
       </c>
       <c r="AJ14" s="9" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="AK14" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AL14" s="8"/>
       <c r="AM14" s="9" t="s">
@@ -7237,7 +7236,7 @@
         <v>55</v>
       </c>
       <c r="AS14" s="9">
-        <v>648173052</v>
+        <v>562827444</v>
       </c>
       <c r="AT14" s="14" t="s">
         <v>55</v>
@@ -7256,7 +7255,7 @@
         <v>58</v>
       </c>
       <c r="AZ14" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="BA14" s="8"/>
       <c r="BB14" s="9" t="s">
@@ -7280,7 +7279,7 @@
         <v>269</v>
       </c>
       <c r="B15" s="12">
-        <v>44626</v>
+        <v>44623</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>43</v>
@@ -7332,13 +7331,13 @@
         <v>48</v>
       </c>
       <c r="T15" s="10">
-        <v>7.9861111111111122E-3</v>
+        <v>6.9328703703703696E-3</v>
       </c>
       <c r="U15" s="11">
-        <v>8.3333333333333332E-3</v>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="V15" s="9">
-        <v>2006</v>
+        <v>2009</v>
       </c>
       <c r="W15" s="9" t="s">
         <v>88</v>
@@ -7380,10 +7379,10 @@
         <v>92</v>
       </c>
       <c r="AJ15" s="9" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="AK15" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AL15" s="8"/>
       <c r="AM15" s="9" t="s">
@@ -7405,7 +7404,7 @@
         <v>55</v>
       </c>
       <c r="AS15" s="9">
-        <v>648144288</v>
+        <v>562827444</v>
       </c>
       <c r="AT15" s="9" t="s">
         <v>55</v>
@@ -7424,7 +7423,7 @@
         <v>58</v>
       </c>
       <c r="AZ15" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="BA15" s="8"/>
       <c r="BB15" s="9" t="s">
@@ -7448,7 +7447,7 @@
         <v>273</v>
       </c>
       <c r="B16" s="12">
-        <v>44626</v>
+        <v>44623</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>43</v>
@@ -7500,13 +7499,13 @@
         <v>48</v>
       </c>
       <c r="T16" s="10">
-        <v>7.9861111111111122E-3</v>
+        <v>6.9328703703703696E-3</v>
       </c>
       <c r="U16" s="11">
-        <v>8.3333333333333332E-3</v>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="V16" s="9">
-        <v>2006</v>
+        <v>2009</v>
       </c>
       <c r="W16" s="9" t="s">
         <v>88</v>
@@ -7548,10 +7547,10 @@
         <v>92</v>
       </c>
       <c r="AJ16" s="9" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="AK16" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AL16" s="8"/>
       <c r="AM16" s="9" t="s">
@@ -7573,7 +7572,7 @@
         <v>55</v>
       </c>
       <c r="AS16" s="9">
-        <v>648173052</v>
+        <v>562735700</v>
       </c>
       <c r="AT16" s="9" t="s">
         <v>55</v>
@@ -7592,7 +7591,7 @@
         <v>58</v>
       </c>
       <c r="AZ16" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="BA16" s="8"/>
       <c r="BB16" s="9" t="s">
@@ -7616,7 +7615,7 @@
         <v>277</v>
       </c>
       <c r="B17" s="12">
-        <v>44626</v>
+        <v>44623</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>43</v>
@@ -7668,13 +7667,13 @@
         <v>48</v>
       </c>
       <c r="T17" s="10">
-        <v>7.9861111111111122E-3</v>
+        <v>6.9328703703703696E-3</v>
       </c>
       <c r="U17" s="11">
-        <v>8.3333333333333332E-3</v>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="V17" s="9">
-        <v>2006</v>
+        <v>2009</v>
       </c>
       <c r="W17" s="9" t="s">
         <v>88</v>
@@ -7716,10 +7715,10 @@
         <v>92</v>
       </c>
       <c r="AJ17" s="9" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="AK17" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AL17" s="8"/>
       <c r="AM17" s="9" t="s">
@@ -7741,7 +7740,7 @@
         <v>55</v>
       </c>
       <c r="AS17" s="9">
-        <v>648173052</v>
+        <v>562827444</v>
       </c>
       <c r="AT17" s="9" t="s">
         <v>55</v>
@@ -7760,7 +7759,7 @@
         <v>58</v>
       </c>
       <c r="AZ17" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="BA17" s="8"/>
       <c r="BB17" s="9" t="s">

</xml_diff>